<commit_message>
Update project plan and estimates
</commit_message>
<xml_diff>
--- a/Documentation/Design/Estimates.xlsx
+++ b/Documentation/Design/Estimates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_git\BedBrigadeNational\Documentation\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54FB9834-00CC-4E25-B819-73D89BCE502E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06D9E202-D5CC-4191-A8B0-3836E811D13A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D27F5AFA-C88C-4A2F-A896-BFED2572A1C7}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{D27F5AFA-C88C-4A2F-A896-BFED2572A1C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Estimates" sheetId="1" r:id="rId1"/>
@@ -521,7 +521,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -541,16 +541,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -598,10 +593,10 @@
       <calculatedColumnFormula>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{E075E6CD-1DFD-47F5-B7CE-6A6F43BA85B6}" name="Completed"/>
-    <tableColumn id="8" xr3:uid="{775079EE-6981-4E34-B3C6-3629C5635AE6}" name="Completed Points" dataDxfId="0">
+    <tableColumn id="8" xr3:uid="{775079EE-6981-4E34-B3C6-3629C5635AE6}" name="Completed Points" dataDxfId="1">
       <calculatedColumnFormula>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{B8125C06-D59F-4CA7-817D-1DFF5C288455}" name="Completed Hours" dataDxfId="1">
+    <tableColumn id="7" xr3:uid="{B8125C06-D59F-4CA7-817D-1DFF5C288455}" name="Completed Hours" dataDxfId="0">
       <calculatedColumnFormula>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -910,22 +905,22 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A106" sqref="A106"/>
+      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="34.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="51.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="51.68359375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.15625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.15625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.15625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.26171875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.83984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -951,7 +946,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -980,7 +975,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1009,7 +1004,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -1038,7 +1033,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -1067,7 +1062,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -1096,7 +1091,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -1125,7 +1120,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -1154,7 +1149,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -1183,7 +1178,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -1212,7 +1207,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -1241,7 +1236,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -1270,7 +1265,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -1299,7 +1294,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -1328,7 +1323,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -1341,7 +1336,7 @@
       <c r="D15" s="3">
         <v>1</v>
       </c>
-      <c r="E15" s="9">
+      <c r="E15" s="3">
         <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
         <v>4</v>
       </c>
@@ -1352,12 +1347,12 @@
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
         <v>1</v>
       </c>
-      <c r="H15" s="10">
+      <c r="H15">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -1374,16 +1369,19 @@
         <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
         <v>8</v>
       </c>
+      <c r="F16" t="b">
+        <v>1</v>
+      </c>
       <c r="G16">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H16">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -1409,7 +1407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -1422,7 +1420,7 @@
       <c r="D18" s="3">
         <v>1</v>
       </c>
-      <c r="E18" s="9">
+      <c r="E18" s="3">
         <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
         <v>4</v>
       </c>
@@ -1430,12 +1428,12 @@
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
         <v>0</v>
       </c>
-      <c r="H18" s="10">
-        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H18">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -1448,7 +1446,7 @@
       <c r="D19" s="3">
         <v>1</v>
       </c>
-      <c r="E19" s="9">
+      <c r="E19" s="3">
         <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
         <v>4</v>
       </c>
@@ -1456,12 +1454,12 @@
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
         <v>0</v>
       </c>
-      <c r="H19" s="10">
-        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H19">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -1474,7 +1472,7 @@
       <c r="D20" s="3">
         <v>1</v>
       </c>
-      <c r="E20" s="9">
+      <c r="E20" s="3">
         <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
         <v>4</v>
       </c>
@@ -1482,12 +1480,12 @@
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
         <v>0</v>
       </c>
-      <c r="H20" s="10">
-        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H20">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -1513,7 +1511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -1539,7 +1537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -1565,7 +1563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -1591,7 +1589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -1617,7 +1615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -1643,7 +1641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -1669,7 +1667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -1695,7 +1693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -1721,7 +1719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -1747,7 +1745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -1773,7 +1771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -1799,7 +1797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -1825,7 +1823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -1851,7 +1849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -1877,7 +1875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -1903,7 +1901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="3">
         <v>36</v>
       </c>
@@ -1929,7 +1927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="3">
         <v>37</v>
       </c>
@@ -1955,7 +1953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="3">
         <v>38</v>
       </c>
@@ -1981,7 +1979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="3">
         <v>39</v>
       </c>
@@ -2007,7 +2005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="3">
         <v>40</v>
       </c>
@@ -2033,7 +2031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="3">
         <v>41</v>
       </c>
@@ -2059,7 +2057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="3">
         <v>42</v>
       </c>
@@ -2085,7 +2083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="3">
         <v>43</v>
       </c>
@@ -2111,7 +2109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="3">
         <v>44</v>
       </c>
@@ -2137,7 +2135,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="3">
         <v>45</v>
       </c>
@@ -2163,7 +2161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="3">
         <v>46</v>
       </c>
@@ -2189,7 +2187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="3">
         <v>47</v>
       </c>
@@ -2215,7 +2213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="3">
         <v>48</v>
       </c>
@@ -2241,7 +2239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="3">
         <v>49</v>
       </c>
@@ -2267,7 +2265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="3">
         <v>50</v>
       </c>
@@ -2293,7 +2291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="3">
         <v>51</v>
       </c>
@@ -2319,7 +2317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="3">
         <v>52</v>
       </c>
@@ -2345,7 +2343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="3">
         <v>53</v>
       </c>
@@ -2371,7 +2369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="3">
         <v>54</v>
       </c>
@@ -2397,7 +2395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="3">
         <v>55</v>
       </c>
@@ -2423,7 +2421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="3">
         <v>56</v>
       </c>
@@ -2449,7 +2447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="3">
         <v>57</v>
       </c>
@@ -2475,7 +2473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="3">
         <v>58</v>
       </c>
@@ -2501,7 +2499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="3">
         <v>59</v>
       </c>
@@ -2527,7 +2525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="3">
         <v>60</v>
       </c>
@@ -2553,7 +2551,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="3">
         <v>61</v>
       </c>
@@ -2579,7 +2577,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="3">
         <v>62</v>
       </c>
@@ -2605,7 +2603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="3">
         <v>63</v>
       </c>
@@ -2631,7 +2629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="3">
         <v>64</v>
       </c>
@@ -2657,7 +2655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="3">
         <v>65</v>
       </c>
@@ -2683,7 +2681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="3">
         <v>66</v>
       </c>
@@ -2709,7 +2707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="3">
         <v>67</v>
       </c>
@@ -2735,7 +2733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="3">
         <v>68</v>
       </c>
@@ -2761,7 +2759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="3">
         <v>69</v>
       </c>
@@ -2787,7 +2785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="3">
         <v>70</v>
       </c>
@@ -2813,7 +2811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" s="3">
         <v>71</v>
       </c>
@@ -2839,7 +2837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="3">
         <v>72</v>
       </c>
@@ -2865,7 +2863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="3">
         <v>73</v>
       </c>
@@ -2891,7 +2889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" s="3">
         <v>74</v>
       </c>
@@ -2917,7 +2915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" s="3">
         <v>75</v>
       </c>
@@ -2943,7 +2941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="3">
         <v>76</v>
       </c>
@@ -2969,7 +2967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" s="3">
         <v>77</v>
       </c>
@@ -2995,7 +2993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="3">
         <v>78</v>
       </c>
@@ -3021,7 +3019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" s="3">
         <v>79</v>
       </c>
@@ -3047,7 +3045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" s="3">
         <v>80</v>
       </c>
@@ -3073,7 +3071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" s="3">
         <v>81</v>
       </c>
@@ -3099,7 +3097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" s="3">
         <v>82</v>
       </c>
@@ -3125,7 +3123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" s="3">
         <v>83</v>
       </c>
@@ -3151,7 +3149,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" s="3">
         <v>84</v>
       </c>
@@ -3177,7 +3175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" s="3">
         <v>85</v>
       </c>
@@ -3203,7 +3201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" s="3">
         <v>86</v>
       </c>
@@ -3229,7 +3227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" s="3">
         <v>87</v>
       </c>
@@ -3255,7 +3253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" s="3">
         <v>88</v>
       </c>
@@ -3281,7 +3279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" s="3">
         <v>89</v>
       </c>
@@ -3307,7 +3305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" s="3">
         <v>90</v>
       </c>
@@ -3333,7 +3331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" s="3">
         <v>91</v>
       </c>
@@ -3359,7 +3357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" s="3">
         <v>92</v>
       </c>
@@ -3385,7 +3383,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" s="3">
         <v>93</v>
       </c>
@@ -3411,7 +3409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" s="3">
         <v>94</v>
       </c>
@@ -3437,7 +3435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" s="3">
         <v>95</v>
       </c>
@@ -3463,7 +3461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" s="6" t="s">
         <v>120</v>
       </c>
@@ -3479,14 +3477,14 @@
       </c>
       <c r="G98" s="4">
         <f>SUM(G2:G97)</f>
-        <v>18</v>
-      </c>
-      <c r="H98" s="14">
+        <v>20</v>
+      </c>
+      <c r="H98">
         <f>SUM(H2:H97)</f>
-        <v>72</v>
-      </c>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" s="6"/>
       <c r="B99" s="4"/>
       <c r="C99" s="4"/>
@@ -3494,27 +3492,27 @@
       <c r="E99" s="5"/>
       <c r="H99" s="4"/>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="B100" s="13">
+      <c r="B100" s="11">
         <f>E98/Resources!B6</f>
         <v>46.25</v>
       </c>
       <c r="E100" s="7"/>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" s="6" t="s">
         <v>132</v>
       </c>
       <c r="B101" s="4">
         <f>(E98-H98)/Resources!B6</f>
-        <v>44</v>
+        <v>43.75</v>
       </c>
       <c r="E101" s="7"/>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" s="6" t="s">
         <v>131</v>
       </c>
@@ -3524,33 +3522,33 @@
       </c>
       <c r="E102" s="7"/>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="B103" s="15">
+      <c r="B103" s="12">
         <f ca="1">TODAY()+ (E101*7)</f>
-        <v>44923</v>
-      </c>
-      <c r="E103" s="11"/>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+        <v>44925</v>
+      </c>
+      <c r="E103" s="9"/>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="B104" s="13">
+      <c r="B104" s="11">
         <f ca="1">G98/B102</f>
-        <v>4.5</v>
-      </c>
-      <c r="G104" s="12"/>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="G104" s="10"/>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" s="6" t="s">
         <v>138</v>
       </c>
       <c r="B105" s="4">
         <f ca="1">H98/B102</f>
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -3570,14 +3568,14 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="3"/>
+    <col min="1" max="1" width="6.578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.83984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.15625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -3588,7 +3586,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3599,7 +3597,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3610,7 +3608,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3621,7 +3619,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <v>5</v>
       </c>
@@ -3632,7 +3630,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <v>8</v>
       </c>
@@ -3656,12 +3654,12 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.15625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>121</v>
       </c>
@@ -3669,7 +3667,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>122</v>
       </c>
@@ -3677,7 +3675,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>123</v>
       </c>
@@ -3685,7 +3683,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>128</v>
       </c>
@@ -3693,7 +3691,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="4" t="s">
         <v>120</v>
       </c>
@@ -3715,12 +3713,12 @@
       <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.68359375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>129</v>
       </c>
@@ -3728,7 +3726,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>130</v>
       </c>

</xml_diff>

<commit_message>
Quality Check Async Methods
</commit_message>
<xml_diff>
--- a/Documentation/Design/Estimates.xlsx
+++ b/Documentation/Design/Estimates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_git\BedBrigadeNational\Documentation\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06D9E202-D5CC-4191-A8B0-3836E811D13A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43F60C7F-6FCD-4E01-9207-4576A654CA8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{D27F5AFA-C88C-4A2F-A896-BFED2572A1C7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D27F5AFA-C88C-4A2F-A896-BFED2572A1C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Estimates" sheetId="1" r:id="rId1"/>
@@ -101,9 +101,6 @@
     <t>Entity Framework Models</t>
   </si>
   <si>
-    <t>Serilog Console, File and Database Logging</t>
-  </si>
-  <si>
     <t>Setup Deployment</t>
   </si>
   <si>
@@ -465,6 +462,9 @@
   </si>
   <si>
     <t>Value</t>
+  </si>
+  <si>
+    <t>Serilog Console, File Logging</t>
   </si>
 </sst>
 </file>
@@ -905,22 +905,22 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
+      <selection pane="bottomLeft" activeCell="B105" sqref="B105"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="51.68359375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.15625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.15625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.15625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.26171875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.83984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="51.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -937,16 +937,16 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>124</v>
+      </c>
+      <c r="G1" t="s">
+        <v>138</v>
+      </c>
+      <c r="H1" t="s">
         <v>125</v>
       </c>
-      <c r="G1" t="s">
-        <v>139</v>
-      </c>
-      <c r="H1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -975,7 +975,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1004,7 +1004,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -1033,7 +1033,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -1062,7 +1062,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -1091,7 +1091,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -1120,7 +1120,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -1149,7 +1149,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -1178,7 +1178,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -1207,7 +1207,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -1236,7 +1236,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -1265,7 +1265,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -1294,7 +1294,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -1323,7 +1323,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -1331,7 +1331,7 @@
         <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D15" s="3">
         <v>1</v>
@@ -1352,7 +1352,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -1381,7 +1381,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -1389,7 +1389,7 @@
         <v>5</v>
       </c>
       <c r="C17" t="s">
-        <v>20</v>
+        <v>141</v>
       </c>
       <c r="D17" s="3">
         <v>2</v>
@@ -1398,16 +1398,19 @@
         <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
         <v>8</v>
       </c>
+      <c r="F17" t="b">
+        <v>1</v>
+      </c>
       <c r="G17">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H17">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -1415,7 +1418,7 @@
         <v>5</v>
       </c>
       <c r="C18" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D18" s="3">
         <v>1</v>
@@ -1433,7 +1436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -1441,7 +1444,7 @@
         <v>5</v>
       </c>
       <c r="C19" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D19" s="3">
         <v>1</v>
@@ -1459,7 +1462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -1467,7 +1470,7 @@
         <v>5</v>
       </c>
       <c r="C20" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D20" s="3">
         <v>1</v>
@@ -1476,16 +1479,19 @@
         <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
         <v>4</v>
       </c>
+      <c r="F20" t="b">
+        <v>1</v>
+      </c>
       <c r="G20">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H20">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -1493,7 +1499,7 @@
         <v>5</v>
       </c>
       <c r="C21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D21" s="3">
         <v>3</v>
@@ -1511,15 +1517,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>21</v>
       </c>
       <c r="B22" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" t="s">
         <v>29</v>
-      </c>
-      <c r="C22" t="s">
-        <v>30</v>
       </c>
       <c r="D22" s="3">
         <v>3</v>
@@ -1537,15 +1543,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D23" s="3">
         <v>2</v>
@@ -1563,15 +1569,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D24" s="3">
         <v>2</v>
@@ -1589,15 +1595,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C25" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D25" s="3">
         <v>2</v>
@@ -1615,15 +1621,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>25</v>
       </c>
       <c r="B26" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" t="s">
         <v>34</v>
-      </c>
-      <c r="C26" t="s">
-        <v>35</v>
       </c>
       <c r="D26" s="3">
         <v>3</v>
@@ -1641,15 +1647,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D27" s="3">
         <v>2</v>
@@ -1667,15 +1673,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D28" s="3">
         <v>3</v>
@@ -1693,15 +1699,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C29" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D29" s="3">
         <v>5</v>
@@ -1719,15 +1725,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D30" s="3">
         <v>5</v>
@@ -1745,15 +1751,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C31" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D31" s="3">
         <v>5</v>
@@ -1771,15 +1777,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C32" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D32" s="3">
         <v>5</v>
@@ -1797,16 +1803,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>32</v>
       </c>
       <c r="B33" t="s">
+        <v>41</v>
+      </c>
+      <c r="C33" t="s">
         <v>42</v>
       </c>
-      <c r="C33" t="s">
-        <v>43</v>
-      </c>
       <c r="D33" s="3">
         <v>5</v>
       </c>
@@ -1823,15 +1829,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C34" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D34" s="3">
         <v>3</v>
@@ -1849,15 +1855,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C35" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D35" s="3">
         <v>2</v>
@@ -1875,15 +1881,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C36" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D36" s="3">
         <v>2</v>
@@ -1901,15 +1907,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C37" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D37" s="3">
         <v>2</v>
@@ -1927,15 +1933,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C38" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D38" s="3">
         <v>1</v>
@@ -1953,15 +1959,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>38</v>
       </c>
       <c r="B39" t="s">
+        <v>48</v>
+      </c>
+      <c r="C39" t="s">
         <v>49</v>
-      </c>
-      <c r="C39" t="s">
-        <v>50</v>
       </c>
       <c r="D39" s="3">
         <v>3</v>
@@ -1979,15 +1985,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C40" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D40" s="3">
         <v>5</v>
@@ -2005,15 +2011,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C41" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D41" s="3">
         <v>2</v>
@@ -2031,15 +2037,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C42" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D42" s="3">
         <v>2</v>
@@ -2057,15 +2063,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C43" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D43" s="3">
         <v>2</v>
@@ -2083,16 +2089,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>43</v>
       </c>
       <c r="B44" t="s">
+        <v>54</v>
+      </c>
+      <c r="C44" t="s">
         <v>55</v>
       </c>
-      <c r="C44" t="s">
-        <v>56</v>
-      </c>
       <c r="D44" s="3">
         <v>2</v>
       </c>
@@ -2109,15 +2115,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C45" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D45" s="3">
         <v>2</v>
@@ -2135,15 +2141,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>45</v>
       </c>
       <c r="B46" t="s">
+        <v>57</v>
+      </c>
+      <c r="C46" t="s">
         <v>58</v>
-      </c>
-      <c r="C46" t="s">
-        <v>59</v>
       </c>
       <c r="D46" s="3">
         <v>3</v>
@@ -2161,15 +2167,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C47" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D47" s="3">
         <v>3</v>
@@ -2187,15 +2193,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C48" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D48" s="3">
         <v>3</v>
@@ -2213,15 +2219,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C49" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D49" s="3">
         <v>5</v>
@@ -2239,15 +2245,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D50" s="3">
         <v>2</v>
@@ -2265,15 +2271,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C51" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D51" s="3">
         <v>2</v>
@@ -2291,15 +2297,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C52" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D52" s="3">
         <v>2</v>
@@ -2317,16 +2323,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>52</v>
       </c>
       <c r="B53" t="s">
+        <v>65</v>
+      </c>
+      <c r="C53" t="s">
         <v>66</v>
       </c>
-      <c r="C53" t="s">
-        <v>67</v>
-      </c>
       <c r="D53" s="3">
         <v>5</v>
       </c>
@@ -2343,15 +2349,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C54" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D54" s="3">
         <v>3</v>
@@ -2369,15 +2375,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C55" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D55" s="3">
         <v>5</v>
@@ -2395,15 +2401,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C56" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D56" s="3">
         <v>2</v>
@@ -2421,16 +2427,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
         <v>56</v>
       </c>
       <c r="B57" t="s">
+        <v>70</v>
+      </c>
+      <c r="C57" t="s">
         <v>71</v>
       </c>
-      <c r="C57" t="s">
-        <v>72</v>
-      </c>
       <c r="D57" s="3">
         <v>5</v>
       </c>
@@ -2447,15 +2453,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C58" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D58" s="3">
         <v>5</v>
@@ -2473,15 +2479,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C59" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D59" s="3">
         <v>5</v>
@@ -2499,15 +2505,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C60" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D60" s="3">
         <v>3</v>
@@ -2525,15 +2531,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C61" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D61" s="3">
         <v>5</v>
@@ -2551,16 +2557,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
         <v>61</v>
       </c>
       <c r="B62" t="s">
+        <v>76</v>
+      </c>
+      <c r="C62" t="s">
         <v>77</v>
       </c>
-      <c r="C62" t="s">
-        <v>78</v>
-      </c>
       <c r="D62" s="3">
         <v>5</v>
       </c>
@@ -2577,15 +2583,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C63" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D63" s="3">
         <v>5</v>
@@ -2603,15 +2609,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C64" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D64" s="3">
         <v>3</v>
@@ -2629,15 +2635,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
         <v>64</v>
       </c>
       <c r="B65" t="s">
+        <v>80</v>
+      </c>
+      <c r="C65" t="s">
         <v>81</v>
-      </c>
-      <c r="C65" t="s">
-        <v>82</v>
       </c>
       <c r="D65" s="3">
         <v>3</v>
@@ -2655,15 +2661,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="3">
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C66" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D66" s="3">
         <v>5</v>
@@ -2681,15 +2687,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C67" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D67" s="3">
         <v>5</v>
@@ -2707,15 +2713,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
         <v>67</v>
       </c>
       <c r="B68" t="s">
+        <v>83</v>
+      </c>
+      <c r="C68" t="s">
         <v>84</v>
-      </c>
-      <c r="C68" t="s">
-        <v>85</v>
       </c>
       <c r="D68" s="3">
         <v>3</v>
@@ -2733,15 +2739,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="3">
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C69" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D69" s="3">
         <v>3</v>
@@ -2759,15 +2765,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="3">
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C70" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D70" s="3">
         <v>5</v>
@@ -2785,15 +2791,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="3">
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C71" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D71" s="3">
         <v>5</v>
@@ -2811,15 +2817,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="3">
         <v>71</v>
       </c>
       <c r="B72" t="s">
+        <v>89</v>
+      </c>
+      <c r="C72" t="s">
         <v>90</v>
-      </c>
-      <c r="C72" t="s">
-        <v>91</v>
       </c>
       <c r="D72" s="3">
         <v>3</v>
@@ -2837,15 +2843,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="3">
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C73" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D73" s="3">
         <v>3</v>
@@ -2863,15 +2869,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="3">
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C74" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D74" s="3">
         <v>3</v>
@@ -2889,15 +2895,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="3">
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C75" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D75" s="3">
         <v>3</v>
@@ -2915,15 +2921,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="3">
         <v>75</v>
       </c>
       <c r="B76" t="s">
+        <v>94</v>
+      </c>
+      <c r="C76" t="s">
         <v>95</v>
-      </c>
-      <c r="C76" t="s">
-        <v>96</v>
       </c>
       <c r="D76" s="3">
         <v>3</v>
@@ -2941,15 +2947,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="3">
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C77" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D77" s="3">
         <v>3</v>
@@ -2967,15 +2973,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="3">
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C78" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D78" s="3">
         <v>3</v>
@@ -2993,15 +2999,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="3">
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C79" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D79" s="3">
         <v>3</v>
@@ -3019,15 +3025,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="3">
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C80" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D80" s="3">
         <v>3</v>
@@ -3045,15 +3051,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="3">
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C81" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D81" s="3">
         <v>2</v>
@@ -3071,16 +3077,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="3">
         <v>81</v>
       </c>
       <c r="B82" t="s">
+        <v>101</v>
+      </c>
+      <c r="C82" t="s">
         <v>102</v>
       </c>
-      <c r="C82" t="s">
-        <v>103</v>
-      </c>
       <c r="D82" s="3">
         <v>2</v>
       </c>
@@ -3097,15 +3103,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="3">
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C83" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D83" s="3">
         <v>2</v>
@@ -3123,15 +3129,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="3">
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C84" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D84" s="3">
         <v>2</v>
@@ -3149,15 +3155,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="3">
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C85" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D85" s="3">
         <v>2</v>
@@ -3175,15 +3181,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="3">
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C86" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D86" s="3">
         <v>2</v>
@@ -3201,15 +3207,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="3">
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C87" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D87" s="3">
         <v>2</v>
@@ -3227,15 +3233,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="3">
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C88" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D88" s="3">
         <v>2</v>
@@ -3253,15 +3259,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="3">
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C89" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D89" s="3">
         <v>5</v>
@@ -3279,15 +3285,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="3">
         <v>89</v>
       </c>
       <c r="B90" t="s">
+        <v>110</v>
+      </c>
+      <c r="C90" t="s">
         <v>111</v>
-      </c>
-      <c r="C90" t="s">
-        <v>112</v>
       </c>
       <c r="D90" s="3">
         <v>3</v>
@@ -3305,15 +3311,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="3">
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C91" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D91" s="3">
         <v>5</v>
@@ -3331,16 +3337,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="3">
         <v>91</v>
       </c>
       <c r="B92" t="s">
+        <v>113</v>
+      </c>
+      <c r="C92" t="s">
         <v>114</v>
       </c>
-      <c r="C92" t="s">
-        <v>115</v>
-      </c>
       <c r="D92" s="3">
         <v>2</v>
       </c>
@@ -3357,15 +3363,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="3">
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C93" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D93" s="3">
         <v>2</v>
@@ -3383,15 +3389,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="3">
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C94" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D94" s="3">
         <v>5</v>
@@ -3409,15 +3415,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="3">
         <v>94</v>
       </c>
       <c r="B95" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C95" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D95" s="3">
         <v>5</v>
@@ -3435,35 +3441,35 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="3">
         <v>95</v>
       </c>
       <c r="B96" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C96" t="s">
+        <v>118</v>
+      </c>
+      <c r="D96" s="3">
+        <v>5</v>
+      </c>
+      <c r="E96" s="3">
+        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
+        <v>32</v>
+      </c>
+      <c r="G96">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="H96">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A98" s="6" t="s">
         <v>119</v>
-      </c>
-      <c r="D96" s="3">
-        <v>5</v>
-      </c>
-      <c r="E96" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
-        <v>32</v>
-      </c>
-      <c r="G96">
-        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
-      </c>
-      <c r="H96">
-        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A98" s="6" t="s">
-        <v>120</v>
       </c>
       <c r="B98" s="4"/>
       <c r="C98" s="4"/>
@@ -3477,14 +3483,14 @@
       </c>
       <c r="G98" s="4">
         <f>SUM(G2:G97)</f>
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="H98">
         <f>SUM(H2:H97)</f>
-        <v>80</v>
-      </c>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="6"/>
       <c r="B99" s="4"/>
       <c r="C99" s="4"/>
@@ -3492,9 +3498,9 @@
       <c r="E99" s="5"/>
       <c r="H99" s="4"/>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B100" s="11">
         <f>E98/Resources!B6</f>
@@ -3502,53 +3508,53 @@
       </c>
       <c r="E100" s="7"/>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B101" s="4">
         <f>(E98-H98)/Resources!B6</f>
-        <v>43.75</v>
+        <v>43.375</v>
       </c>
       <c r="E101" s="7"/>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B102" s="4">
         <f ca="1">FLOOR(((TODAY()-Variables!B2)/7),1)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E102" s="7"/>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B103" s="12">
-        <f ca="1">TODAY()+ (E101*7)</f>
-        <v>44925</v>
+        <f ca="1">TODAY()+ (B101*7)</f>
+        <v>45231.625</v>
       </c>
       <c r="E103" s="9"/>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B104" s="11">
         <f ca="1">G98/B102</f>
-        <v>5</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="G104" s="10"/>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B105" s="4">
         <f ca="1">H98/B102</f>
-        <v>20</v>
+        <v>18.399999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -3568,74 +3574,74 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.83984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.15625" style="3"/>
+    <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>25</v>
       </c>
       <c r="C2" s="3">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" s="3">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C4" s="3">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C5" s="3">
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C6" s="3">
         <v>64</v>
@@ -3654,46 +3660,46 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="38.15625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>121</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" t="s">
+      <c r="B2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>122</v>
-      </c>
-      <c r="B2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="s">
-        <v>123</v>
       </c>
       <c r="B3">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B4">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B6" s="4">
         <f>SUM(B2:B4)</f>
@@ -3713,22 +3719,22 @@
       <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.68359375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>129</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" t="s">
-        <v>130</v>
       </c>
       <c r="B2" s="8">
         <v>44892</v>

</xml_diff>

<commit_message>
Code quality check razor pages
</commit_message>
<xml_diff>
--- a/Documentation/Design/Estimates.xlsx
+++ b/Documentation/Design/Estimates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_git\BedBrigadeNational\Documentation\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43F60C7F-6FCD-4E01-9207-4576A654CA8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A841A77-DFBF-4533-B301-873D03962B16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D27F5AFA-C88C-4A2F-A896-BFED2572A1C7}"/>
   </bookViews>
@@ -904,8 +904,8 @@
   <dimension ref="A1:H105"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B105" sqref="B105"/>
+      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1453,13 +1453,16 @@
         <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
         <v>4</v>
       </c>
+      <c r="F19" t="b">
+        <v>1</v>
+      </c>
       <c r="G19">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H19">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -3483,11 +3486,11 @@
       </c>
       <c r="G98" s="4">
         <f>SUM(G2:G97)</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H98">
         <f>SUM(H2:H97)</f>
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
@@ -3514,7 +3517,7 @@
       </c>
       <c r="B101" s="4">
         <f>(E98-H98)/Resources!B6</f>
-        <v>43.375</v>
+        <v>43.25</v>
       </c>
       <c r="E101" s="7"/>
     </row>
@@ -3534,7 +3537,7 @@
       </c>
       <c r="B103" s="12">
         <f ca="1">TODAY()+ (B101*7)</f>
-        <v>45231.625</v>
+        <v>45231.75</v>
       </c>
       <c r="E103" s="9"/>
     </row>
@@ -3544,7 +3547,7 @@
       </c>
       <c r="B104" s="11">
         <f ca="1">G98/B102</f>
-        <v>4.5999999999999996</v>
+        <v>4.8</v>
       </c>
       <c r="G104" s="10"/>
     </row>
@@ -3554,7 +3557,7 @@
       </c>
       <c r="B105" s="4">
         <f ca="1">H98/B102</f>
-        <v>18.399999999999999</v>
+        <v>19.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Getting Started to include Gold License. Update Project Plan and Estimates.
</commit_message>
<xml_diff>
--- a/Documentation/Design/Estimates.xlsx
+++ b/Documentation/Design/Estimates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_git\BedBrigadeNational\Documentation\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F564163-250A-47A2-9581-E14F0D063FE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC610649-9682-4E2D-A867-35E48510554D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D27F5AFA-C88C-4A2F-A896-BFED2572A1C7}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D27F5AFA-C88C-4A2F-A896-BFED2572A1C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Estimates" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="145">
   <si>
     <t>Epic</t>
   </si>
@@ -402,12 +402,6 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Greg</t>
-  </si>
-  <si>
-    <t>James</t>
-  </si>
-  <si>
     <t>Dedicated Development Hours Per Week</t>
   </si>
   <si>
@@ -420,9 +414,6 @@
     <t>Total Weeks</t>
   </si>
   <si>
-    <t>Anna</t>
-  </si>
-  <si>
     <t>Variable</t>
   </si>
   <si>
@@ -435,9 +426,6 @@
     <t>Estimated Completion Date</t>
   </si>
   <si>
-    <t>Create Theme Using Syncfusion Theme Studio for Blazor</t>
-  </si>
-  <si>
     <t>Code Quality Check Razor Pages</t>
   </si>
   <si>
@@ -475,6 +463,18 @@
   </si>
   <si>
     <t>Project Start Date</t>
+  </si>
+  <si>
+    <t>Greg Finzer</t>
+  </si>
+  <si>
+    <t>James MacIvor</t>
+  </si>
+  <si>
+    <t>Mike Chafin</t>
+  </si>
+  <si>
+    <t>Val Skordin</t>
   </si>
 </sst>
 </file>
@@ -531,7 +531,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -557,11 +557,16 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="6">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -574,10 +579,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -596,20 +597,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{20A5C34A-BA74-4618-9527-C8C5A4B15239}" name="Table1" displayName="Table1" ref="A1:G89" totalsRowShown="0">
-  <autoFilter ref="A1:G89" xr:uid="{20A5C34A-BA74-4618-9527-C8C5A4B15239}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{20A5C34A-BA74-4618-9527-C8C5A4B15239}" name="Table1" displayName="Table1" ref="A1:G96" totalsRowShown="0">
+  <autoFilter ref="A1:G96" xr:uid="{20A5C34A-BA74-4618-9527-C8C5A4B15239}"/>
   <tableColumns count="7">
     <tableColumn id="2" xr3:uid="{8122BCC0-A9A0-4E8A-97F8-809454E87965}" name="Epic"/>
     <tableColumn id="3" xr3:uid="{62273C57-4035-404E-BD7F-DBE541848AF0}" name="Story"/>
     <tableColumn id="4" xr3:uid="{F83CC626-5103-462B-9E71-70FF58ECD672}" name="Points" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{32A1D275-1575-4B11-A22D-5A36CD923379}" name="Estimated Hours" dataDxfId="4">
-      <calculatedColumnFormula>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</calculatedColumnFormula>
+    <tableColumn id="5" xr3:uid="{32A1D275-1575-4B11-A22D-5A36CD923379}" name="Estimated Hours" dataDxfId="0">
+      <calculatedColumnFormula>VLOOKUP(C2,Points!$A$1:$C$6,3,FALSE)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{E075E6CD-1DFD-47F5-B7CE-6A6F43BA85B6}" name="Completed"/>
-    <tableColumn id="8" xr3:uid="{775079EE-6981-4E34-B3C6-3629C5635AE6}" name="Completed Points" dataDxfId="3">
+    <tableColumn id="8" xr3:uid="{775079EE-6981-4E34-B3C6-3629C5635AE6}" name="Completed Points" dataDxfId="4">
       <calculatedColumnFormula>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{B8125C06-D59F-4CA7-817D-1DFF5C288455}" name="Completed Hours" dataDxfId="2">
+    <tableColumn id="7" xr3:uid="{B8125C06-D59F-4CA7-817D-1DFF5C288455}" name="Completed Hours" dataDxfId="3">
       <calculatedColumnFormula>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -618,15 +619,13 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{462FB8B6-867C-41A1-BFD9-9F5A89B19647}" name="Table2" displayName="Table2" ref="A1:G9" totalsRowShown="0">
-  <autoFilter ref="A1:G9" xr:uid="{462FB8B6-867C-41A1-BFD9-9F5A89B19647}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{462FB8B6-867C-41A1-BFD9-9F5A89B19647}" name="Table2" displayName="Table2" ref="A1:G2" totalsRowShown="0">
+  <autoFilter ref="A1:G2" xr:uid="{462FB8B6-867C-41A1-BFD9-9F5A89B19647}"/>
   <tableColumns count="7">
     <tableColumn id="2" xr3:uid="{31CB5B43-DDC0-45F7-94FE-8435C1D008DA}" name="Epic"/>
     <tableColumn id="3" xr3:uid="{E8134CEE-EEF4-4605-A21F-CFF015B23BA2}" name="Story"/>
-    <tableColumn id="4" xr3:uid="{A8E050D4-AAEC-4516-ABB3-A0C110009E2F}" name="Points" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{AD6AC57F-E07B-42DB-850E-DEA524AE6E46}" name="Estimated Hours" dataDxfId="0">
-      <calculatedColumnFormula>VLOOKUP(C2,Points!$A$1:$C$6,3,FALSE)</calculatedColumnFormula>
-    </tableColumn>
+    <tableColumn id="4" xr3:uid="{A8E050D4-AAEC-4516-ABB3-A0C110009E2F}" name="Points" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{AD6AC57F-E07B-42DB-850E-DEA524AE6E46}" name="Estimated Hours" dataDxfId="1"/>
     <tableColumn id="6" xr3:uid="{86F5B27A-D198-4848-ADB6-A7BEFFDB816F}" name="Completed"/>
     <tableColumn id="7" xr3:uid="{2398D599-5A1D-4B6E-8A23-79F4063944CE}" name="Completed Points"/>
     <tableColumn id="8" xr3:uid="{C13FCCDE-FC9C-48C6-AE8F-48A44BF6C3D4}" name="Completed Hours"/>
@@ -924,7 +923,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -932,11 +931,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F9D3302-E5F0-4E5C-9EB3-B74DDF37DF9D}">
-  <dimension ref="A1:G99"/>
+  <dimension ref="A1:G106"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="B106" sqref="B106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -964,13 +963,13 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F1" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="G1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -984,7 +983,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
+        <f>VLOOKUP(C2,Points!$A$1:$C$6,3,FALSE)</f>
         <v>4</v>
       </c>
       <c r="E2" t="b">
@@ -1010,7 +1009,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
+        <f>VLOOKUP(C3,Points!$A$1:$C$6,3,FALSE)</f>
         <v>4</v>
       </c>
       <c r="E3" t="b">
@@ -1036,7 +1035,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
+        <f>VLOOKUP(C4,Points!$A$1:$C$6,3,FALSE)</f>
         <v>4</v>
       </c>
       <c r="E4" t="b">
@@ -1062,7 +1061,7 @@
         <v>1</v>
       </c>
       <c r="D5" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
+        <f>VLOOKUP(C5,Points!$A$1:$C$6,3,FALSE)</f>
         <v>4</v>
       </c>
       <c r="E5" t="b">
@@ -1088,7 +1087,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
+        <f>VLOOKUP(C6,Points!$A$1:$C$6,3,FALSE)</f>
         <v>4</v>
       </c>
       <c r="E6" t="b">
@@ -1114,7 +1113,7 @@
         <v>1</v>
       </c>
       <c r="D7" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
+        <f>VLOOKUP(C7,Points!$A$1:$C$6,3,FALSE)</f>
         <v>4</v>
       </c>
       <c r="E7" t="b">
@@ -1140,7 +1139,7 @@
         <v>2</v>
       </c>
       <c r="D8" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
+        <f>VLOOKUP(C8,Points!$A$1:$C$6,3,FALSE)</f>
         <v>8</v>
       </c>
       <c r="E8" t="b">
@@ -1166,7 +1165,7 @@
         <v>2</v>
       </c>
       <c r="D9" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
+        <f>VLOOKUP(C9,Points!$A$1:$C$6,3,FALSE)</f>
         <v>8</v>
       </c>
       <c r="E9" t="b">
@@ -1192,7 +1191,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
+        <f>VLOOKUP(C10,Points!$A$1:$C$6,3,FALSE)</f>
         <v>4</v>
       </c>
       <c r="E10" t="b">
@@ -1218,7 +1217,7 @@
         <v>1</v>
       </c>
       <c r="D11" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
+        <f>VLOOKUP(C11,Points!$A$1:$C$6,3,FALSE)</f>
         <v>4</v>
       </c>
       <c r="E11" t="b">
@@ -1244,7 +1243,7 @@
         <v>2</v>
       </c>
       <c r="D12" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
+        <f>VLOOKUP(C12,Points!$A$1:$C$6,3,FALSE)</f>
         <v>8</v>
       </c>
       <c r="E12" t="b">
@@ -1270,7 +1269,7 @@
         <v>1</v>
       </c>
       <c r="D13" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
+        <f>VLOOKUP(C13,Points!$A$1:$C$6,3,FALSE)</f>
         <v>4</v>
       </c>
       <c r="E13" t="b">
@@ -1296,7 +1295,7 @@
         <v>2</v>
       </c>
       <c r="D14" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
+        <f>VLOOKUP(C14,Points!$A$1:$C$6,3,FALSE)</f>
         <v>8</v>
       </c>
       <c r="E14" t="b">
@@ -1316,13 +1315,13 @@
         <v>4</v>
       </c>
       <c r="B15" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C15" s="3">
         <v>1</v>
       </c>
       <c r="D15" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
+        <f>VLOOKUP(C15,Points!$A$1:$C$6,3,FALSE)</f>
         <v>4</v>
       </c>
       <c r="E15" t="b">
@@ -1348,7 +1347,7 @@
         <v>2</v>
       </c>
       <c r="D16" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
+        <f>VLOOKUP(C16,Points!$A$1:$C$6,3,FALSE)</f>
         <v>8</v>
       </c>
       <c r="E16" t="b">
@@ -1368,13 +1367,13 @@
         <v>4</v>
       </c>
       <c r="B17" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C17" s="3">
         <v>2</v>
       </c>
       <c r="D17" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
+        <f>VLOOKUP(C17,Points!$A$1:$C$6,3,FALSE)</f>
         <v>8</v>
       </c>
       <c r="E17" t="b">
@@ -1394,22 +1393,25 @@
         <v>4</v>
       </c>
       <c r="B18" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C18" s="3">
         <v>1</v>
       </c>
       <c r="D18" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
-        <v>4</v>
+        <f>VLOOKUP(C18,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="E18" t="b">
+        <v>1</v>
       </c>
       <c r="F18">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G18">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1417,13 +1419,13 @@
         <v>4</v>
       </c>
       <c r="B19" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C19" s="3">
         <v>1</v>
       </c>
       <c r="D19" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
+        <f>VLOOKUP(C19,Points!$A$1:$C$6,3,FALSE)</f>
         <v>4</v>
       </c>
       <c r="E19" t="b">
@@ -1443,48 +1445,51 @@
         <v>4</v>
       </c>
       <c r="B20" t="s">
-        <v>133</v>
+        <v>19</v>
       </c>
       <c r="C20" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D20" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
-        <v>4</v>
+        <f>VLOOKUP(C20,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>16</v>
       </c>
       <c r="E20" t="b">
         <v>1</v>
       </c>
       <c r="F20">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G20">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>4</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="B21" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="C21" s="3">
         <v>3</v>
       </c>
       <c r="D21" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
+        <f>VLOOKUP(C21,Points!$A$1:$C$6,3,FALSE)</f>
         <v>16</v>
       </c>
+      <c r="E21" t="b">
+        <v>1</v>
+      </c>
       <c r="F21">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G21">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1492,14 +1497,14 @@
         <v>27</v>
       </c>
       <c r="B22" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C22" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D22" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
-        <v>16</v>
+        <f>VLOOKUP(C22,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>8</v>
       </c>
       <c r="F22">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
@@ -1515,13 +1520,13 @@
         <v>27</v>
       </c>
       <c r="B23" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C23" s="3">
         <v>2</v>
       </c>
       <c r="D23" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
+        <f>VLOOKUP(C23,Points!$A$1:$C$6,3,FALSE)</f>
         <v>8</v>
       </c>
       <c r="F23">
@@ -1538,13 +1543,13 @@
         <v>27</v>
       </c>
       <c r="B24" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C24" s="3">
         <v>2</v>
       </c>
       <c r="D24" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
+        <f>VLOOKUP(C24,Points!$A$1:$C$6,3,FALSE)</f>
         <v>8</v>
       </c>
       <c r="F24">
@@ -1558,17 +1563,17 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B25" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C25" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D25" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
-        <v>8</v>
+        <f>VLOOKUP(C25,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>16</v>
       </c>
       <c r="F25">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
@@ -1584,22 +1589,25 @@
         <v>32</v>
       </c>
       <c r="B26" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C26" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D26" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
-        <v>16</v>
+        <f>VLOOKUP(C26,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>8</v>
+      </c>
+      <c r="E26" t="b">
+        <v>1</v>
       </c>
       <c r="F26">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G26">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1607,14 +1615,14 @@
         <v>32</v>
       </c>
       <c r="B27" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C27" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D27" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
-        <v>8</v>
+        <f>VLOOKUP(C27,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>16</v>
       </c>
       <c r="F27">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
@@ -1630,14 +1638,14 @@
         <v>32</v>
       </c>
       <c r="B28" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C28" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D28" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
-        <v>16</v>
+        <f>VLOOKUP(C28,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>32</v>
       </c>
       <c r="F28">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
@@ -1653,13 +1661,13 @@
         <v>32</v>
       </c>
       <c r="B29" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C29" s="3">
         <v>5</v>
       </c>
       <c r="D29" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
+        <f>VLOOKUP(C29,Points!$A$1:$C$6,3,FALSE)</f>
         <v>32</v>
       </c>
       <c r="F29">
@@ -1676,13 +1684,13 @@
         <v>32</v>
       </c>
       <c r="B30" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C30" s="3">
         <v>5</v>
       </c>
       <c r="D30" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
+        <f>VLOOKUP(C30,Points!$A$1:$C$6,3,FALSE)</f>
         <v>32</v>
       </c>
       <c r="F30">
@@ -1699,13 +1707,13 @@
         <v>32</v>
       </c>
       <c r="B31" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C31" s="3">
         <v>5</v>
       </c>
       <c r="D31" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
+        <f>VLOOKUP(C31,Points!$A$1:$C$6,3,FALSE)</f>
         <v>32</v>
       </c>
       <c r="F31">
@@ -1719,16 +1727,16 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="B32" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C32" s="3">
         <v>5</v>
       </c>
       <c r="D32" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
+        <f>VLOOKUP(C32,Points!$A$1:$C$6,3,FALSE)</f>
         <v>32</v>
       </c>
       <c r="F32">
@@ -1745,14 +1753,14 @@
         <v>40</v>
       </c>
       <c r="B33" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C33" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D33" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
-        <v>32</v>
+        <f>VLOOKUP(C33,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>16</v>
       </c>
       <c r="F33">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
@@ -1768,14 +1776,14 @@
         <v>40</v>
       </c>
       <c r="B34" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C34" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D34" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
-        <v>16</v>
+        <f>VLOOKUP(C34,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>8</v>
       </c>
       <c r="F34">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
@@ -1791,13 +1799,13 @@
         <v>40</v>
       </c>
       <c r="B35" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C35" s="3">
         <v>2</v>
       </c>
       <c r="D35" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
+        <f>VLOOKUP(C35,Points!$A$1:$C$6,3,FALSE)</f>
         <v>8</v>
       </c>
       <c r="F35">
@@ -1814,13 +1822,13 @@
         <v>40</v>
       </c>
       <c r="B36" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C36" s="3">
         <v>2</v>
       </c>
       <c r="D36" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
+        <f>VLOOKUP(C36,Points!$A$1:$C$6,3,FALSE)</f>
         <v>8</v>
       </c>
       <c r="F36">
@@ -1837,14 +1845,14 @@
         <v>40</v>
       </c>
       <c r="B37" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C37" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D37" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
-        <v>8</v>
+        <f>VLOOKUP(C37,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>4</v>
       </c>
       <c r="F37">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
@@ -1857,17 +1865,17 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="B38" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C38" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D38" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
-        <v>4</v>
+        <f>VLOOKUP(C38,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>16</v>
       </c>
       <c r="F38">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
@@ -1883,14 +1891,14 @@
         <v>47</v>
       </c>
       <c r="B39" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C39" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D39" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
-        <v>16</v>
+        <f>VLOOKUP(C39,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>32</v>
       </c>
       <c r="F39">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
@@ -1906,14 +1914,14 @@
         <v>47</v>
       </c>
       <c r="B40" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C40" s="3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D40" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
-        <v>32</v>
+        <f>VLOOKUP(C40,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>8</v>
       </c>
       <c r="F40">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
@@ -1929,13 +1937,13 @@
         <v>47</v>
       </c>
       <c r="B41" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C41" s="3">
         <v>2</v>
       </c>
       <c r="D41" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
+        <f>VLOOKUP(C41,Points!$A$1:$C$6,3,FALSE)</f>
         <v>8</v>
       </c>
       <c r="F41">
@@ -1952,13 +1960,13 @@
         <v>47</v>
       </c>
       <c r="B42" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C42" s="3">
         <v>2</v>
       </c>
       <c r="D42" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
+        <f>VLOOKUP(C42,Points!$A$1:$C$6,3,FALSE)</f>
         <v>8</v>
       </c>
       <c r="F42">
@@ -1972,16 +1980,16 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="B43" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C43" s="3">
         <v>2</v>
       </c>
       <c r="D43" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
+        <f>VLOOKUP(C43,Points!$A$1:$C$6,3,FALSE)</f>
         <v>8</v>
       </c>
       <c r="F43">
@@ -1998,13 +2006,13 @@
         <v>53</v>
       </c>
       <c r="B44" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C44" s="3">
         <v>2</v>
       </c>
       <c r="D44" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
+        <f>VLOOKUP(C44,Points!$A$1:$C$6,3,FALSE)</f>
         <v>8</v>
       </c>
       <c r="F44">
@@ -2018,17 +2026,17 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B45" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C45" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D45" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
-        <v>8</v>
+        <f>VLOOKUP(C45,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>16</v>
       </c>
       <c r="F45">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
@@ -2044,13 +2052,13 @@
         <v>56</v>
       </c>
       <c r="B46" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C46" s="3">
         <v>3</v>
       </c>
       <c r="D46" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
+        <f>VLOOKUP(C46,Points!$A$1:$C$6,3,FALSE)</f>
         <v>16</v>
       </c>
       <c r="F46">
@@ -2067,13 +2075,13 @@
         <v>56</v>
       </c>
       <c r="B47" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C47" s="3">
         <v>3</v>
       </c>
       <c r="D47" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
+        <f>VLOOKUP(C47,Points!$A$1:$C$6,3,FALSE)</f>
         <v>16</v>
       </c>
       <c r="F47">
@@ -2090,14 +2098,14 @@
         <v>56</v>
       </c>
       <c r="B48" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C48" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D48" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
-        <v>16</v>
+        <f>VLOOKUP(C48,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>32</v>
       </c>
       <c r="F48">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
@@ -2113,14 +2121,14 @@
         <v>56</v>
       </c>
       <c r="B49" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C49" s="3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D49" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
-        <v>32</v>
+        <f>VLOOKUP(C49,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>8</v>
       </c>
       <c r="F49">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
@@ -2136,13 +2144,13 @@
         <v>56</v>
       </c>
       <c r="B50" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C50" s="3">
         <v>2</v>
       </c>
       <c r="D50" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
+        <f>VLOOKUP(C50,Points!$A$1:$C$6,3,FALSE)</f>
         <v>8</v>
       </c>
       <c r="F50">
@@ -2159,13 +2167,13 @@
         <v>56</v>
       </c>
       <c r="B51" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C51" s="3">
         <v>2</v>
       </c>
       <c r="D51" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
+        <f>VLOOKUP(C51,Points!$A$1:$C$6,3,FALSE)</f>
         <v>8</v>
       </c>
       <c r="F51">
@@ -2179,17 +2187,17 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="B52" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C52" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D52" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
-        <v>8</v>
+        <f>VLOOKUP(C52,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>32</v>
       </c>
       <c r="F52">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
@@ -2205,14 +2213,14 @@
         <v>64</v>
       </c>
       <c r="B53" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C53" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D53" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
-        <v>32</v>
+        <f>VLOOKUP(C53,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>16</v>
       </c>
       <c r="F53">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
@@ -2228,14 +2236,14 @@
         <v>64</v>
       </c>
       <c r="B54" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C54" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D54" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
-        <v>16</v>
+        <f>VLOOKUP(C54,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>32</v>
       </c>
       <c r="F54">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
@@ -2251,14 +2259,14 @@
         <v>64</v>
       </c>
       <c r="B55" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C55" s="3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D55" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
-        <v>32</v>
+        <f>VLOOKUP(C55,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>8</v>
       </c>
       <c r="F55">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
@@ -2271,17 +2279,17 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="B56" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C56" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D56" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
-        <v>8</v>
+        <f>VLOOKUP(C56,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>32</v>
       </c>
       <c r="F56">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
@@ -2297,13 +2305,13 @@
         <v>69</v>
       </c>
       <c r="B57" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C57" s="3">
         <v>5</v>
       </c>
       <c r="D57" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
+        <f>VLOOKUP(C57,Points!$A$1:$C$6,3,FALSE)</f>
         <v>32</v>
       </c>
       <c r="F57">
@@ -2320,13 +2328,13 @@
         <v>69</v>
       </c>
       <c r="B58" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C58" s="3">
         <v>5</v>
       </c>
       <c r="D58" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
+        <f>VLOOKUP(C58,Points!$A$1:$C$6,3,FALSE)</f>
         <v>32</v>
       </c>
       <c r="F58">
@@ -2343,14 +2351,14 @@
         <v>69</v>
       </c>
       <c r="B59" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C59" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D59" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
-        <v>32</v>
+        <f>VLOOKUP(C59,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>16</v>
       </c>
       <c r="F59">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
@@ -2366,14 +2374,14 @@
         <v>69</v>
       </c>
       <c r="B60" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C60" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D60" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
-        <v>16</v>
+        <f>VLOOKUP(C60,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>32</v>
       </c>
       <c r="F60">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
@@ -2386,16 +2394,16 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="B61" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C61" s="3">
         <v>5</v>
       </c>
       <c r="D61" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
+        <f>VLOOKUP(C61,Points!$A$1:$C$6,3,FALSE)</f>
         <v>32</v>
       </c>
       <c r="F61">
@@ -2412,13 +2420,13 @@
         <v>75</v>
       </c>
       <c r="B62" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C62" s="3">
         <v>5</v>
       </c>
       <c r="D62" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
+        <f>VLOOKUP(C62,Points!$A$1:$C$6,3,FALSE)</f>
         <v>32</v>
       </c>
       <c r="F62">
@@ -2435,14 +2443,14 @@
         <v>75</v>
       </c>
       <c r="B63" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C63" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D63" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
-        <v>32</v>
+        <f>VLOOKUP(C63,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>16</v>
       </c>
       <c r="F63">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
@@ -2455,16 +2463,16 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="B64" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C64" s="3">
         <v>3</v>
       </c>
       <c r="D64" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
+        <f>VLOOKUP(C64,Points!$A$1:$C$6,3,FALSE)</f>
         <v>16</v>
       </c>
       <c r="F64">
@@ -2481,14 +2489,14 @@
         <v>79</v>
       </c>
       <c r="B65" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C65" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D65" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
-        <v>16</v>
+        <f>VLOOKUP(C65,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>32</v>
       </c>
       <c r="F65">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
@@ -2501,16 +2509,16 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B66" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C66" s="3">
         <v>5</v>
       </c>
       <c r="D66" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
+        <f>VLOOKUP(C66,Points!$A$1:$C$6,3,FALSE)</f>
         <v>32</v>
       </c>
       <c r="F66">
@@ -2527,14 +2535,14 @@
         <v>82</v>
       </c>
       <c r="B67" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C67" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D67" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
-        <v>32</v>
+        <f>VLOOKUP(C67,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>16</v>
       </c>
       <c r="F67">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
@@ -2550,13 +2558,13 @@
         <v>82</v>
       </c>
       <c r="B68" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C68" s="3">
         <v>3</v>
       </c>
       <c r="D68" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
+        <f>VLOOKUP(C68,Points!$A$1:$C$6,3,FALSE)</f>
         <v>16</v>
       </c>
       <c r="F68">
@@ -2573,14 +2581,14 @@
         <v>82</v>
       </c>
       <c r="B69" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C69" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D69" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
-        <v>16</v>
+        <f>VLOOKUP(C69,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>32</v>
       </c>
       <c r="F69">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
@@ -2596,13 +2604,13 @@
         <v>82</v>
       </c>
       <c r="B70" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C70" s="3">
         <v>5</v>
       </c>
       <c r="D70" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
+        <f>VLOOKUP(C70,Points!$A$1:$C$6,3,FALSE)</f>
         <v>32</v>
       </c>
       <c r="F70">
@@ -2616,17 +2624,17 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="B71" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C71" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D71" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
-        <v>32</v>
+        <f>VLOOKUP(C71,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>16</v>
       </c>
       <c r="F71">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
@@ -2642,13 +2650,13 @@
         <v>88</v>
       </c>
       <c r="B72" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C72" s="3">
         <v>3</v>
       </c>
       <c r="D72" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
+        <f>VLOOKUP(C72,Points!$A$1:$C$6,3,FALSE)</f>
         <v>16</v>
       </c>
       <c r="F72">
@@ -2665,13 +2673,13 @@
         <v>88</v>
       </c>
       <c r="B73" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C73" s="3">
         <v>3</v>
       </c>
       <c r="D73" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
+        <f>VLOOKUP(C73,Points!$A$1:$C$6,3,FALSE)</f>
         <v>16</v>
       </c>
       <c r="F73">
@@ -2688,13 +2696,13 @@
         <v>88</v>
       </c>
       <c r="B74" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C74" s="3">
         <v>3</v>
       </c>
       <c r="D74" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
+        <f>VLOOKUP(C74,Points!$A$1:$C$6,3,FALSE)</f>
         <v>16</v>
       </c>
       <c r="F74">
@@ -2708,16 +2716,16 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="B75" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C75" s="3">
         <v>3</v>
       </c>
       <c r="D75" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
+        <f>VLOOKUP(C75,Points!$A$1:$C$6,3,FALSE)</f>
         <v>16</v>
       </c>
       <c r="F75">
@@ -2734,13 +2742,13 @@
         <v>93</v>
       </c>
       <c r="B76" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C76" s="3">
         <v>3</v>
       </c>
       <c r="D76" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
+        <f>VLOOKUP(C76,Points!$A$1:$C$6,3,FALSE)</f>
         <v>16</v>
       </c>
       <c r="F76">
@@ -2757,13 +2765,13 @@
         <v>93</v>
       </c>
       <c r="B77" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C77" s="3">
         <v>3</v>
       </c>
       <c r="D77" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
+        <f>VLOOKUP(C77,Points!$A$1:$C$6,3,FALSE)</f>
         <v>16</v>
       </c>
       <c r="F77">
@@ -2780,13 +2788,13 @@
         <v>93</v>
       </c>
       <c r="B78" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C78" s="3">
         <v>3</v>
       </c>
       <c r="D78" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
+        <f>VLOOKUP(C78,Points!$A$1:$C$6,3,FALSE)</f>
         <v>16</v>
       </c>
       <c r="F78">
@@ -2803,13 +2811,13 @@
         <v>93</v>
       </c>
       <c r="B79" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C79" s="3">
         <v>3</v>
       </c>
       <c r="D79" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
+        <f>VLOOKUP(C79,Points!$A$1:$C$6,3,FALSE)</f>
         <v>16</v>
       </c>
       <c r="F79">
@@ -2826,14 +2834,14 @@
         <v>93</v>
       </c>
       <c r="B80" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C80" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D80" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
-        <v>16</v>
+        <f>VLOOKUP(C80,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>8</v>
       </c>
       <c r="F80">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
@@ -2846,16 +2854,16 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="B81" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C81" s="3">
         <v>2</v>
       </c>
       <c r="D81" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
+        <f>VLOOKUP(C81,Points!$A$1:$C$6,3,FALSE)</f>
         <v>8</v>
       </c>
       <c r="F81">
@@ -2872,13 +2880,13 @@
         <v>100</v>
       </c>
       <c r="B82" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C82" s="3">
         <v>2</v>
       </c>
       <c r="D82" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
+        <f>VLOOKUP(C82,Points!$A$1:$C$6,3,FALSE)</f>
         <v>8</v>
       </c>
       <c r="F82">
@@ -2895,13 +2903,13 @@
         <v>100</v>
       </c>
       <c r="B83" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C83" s="3">
         <v>2</v>
       </c>
       <c r="D83" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
+        <f>VLOOKUP(C83,Points!$A$1:$C$6,3,FALSE)</f>
         <v>8</v>
       </c>
       <c r="F83">
@@ -2918,13 +2926,13 @@
         <v>100</v>
       </c>
       <c r="B84" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C84" s="3">
         <v>2</v>
       </c>
       <c r="D84" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
+        <f>VLOOKUP(C84,Points!$A$1:$C$6,3,FALSE)</f>
         <v>8</v>
       </c>
       <c r="F84">
@@ -2941,13 +2949,13 @@
         <v>100</v>
       </c>
       <c r="B85" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C85" s="3">
         <v>2</v>
       </c>
       <c r="D85" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
+        <f>VLOOKUP(C85,Points!$A$1:$C$6,3,FALSE)</f>
         <v>8</v>
       </c>
       <c r="F85">
@@ -2964,13 +2972,13 @@
         <v>100</v>
       </c>
       <c r="B86" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C86" s="3">
         <v>2</v>
       </c>
       <c r="D86" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
+        <f>VLOOKUP(C86,Points!$A$1:$C$6,3,FALSE)</f>
         <v>8</v>
       </c>
       <c r="F86">
@@ -2987,13 +2995,13 @@
         <v>100</v>
       </c>
       <c r="B87" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C87" s="3">
         <v>2</v>
       </c>
       <c r="D87" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
+        <f>VLOOKUP(C87,Points!$A$1:$C$6,3,FALSE)</f>
         <v>8</v>
       </c>
       <c r="F87">
@@ -3007,146 +3015,307 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="B88" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C88" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D88" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
-        <v>8</v>
-      </c>
-      <c r="F88">
-        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
-      </c>
-      <c r="G88">
+        <f>VLOOKUP(C88,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>32</v>
+      </c>
+      <c r="F88" s="13">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="G88" s="13">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
+        <v>109</v>
+      </c>
+      <c r="B89" t="s">
+        <v>110</v>
+      </c>
+      <c r="C89" s="3">
+        <v>3</v>
+      </c>
+      <c r="D89" s="3">
+        <f>VLOOKUP(C89,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>16</v>
+      </c>
+      <c r="F89" s="13">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="G89" s="13">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>109</v>
+      </c>
+      <c r="B90" t="s">
+        <v>111</v>
+      </c>
+      <c r="C90" s="3">
+        <v>5</v>
+      </c>
+      <c r="D90" s="3">
+        <f>VLOOKUP(C90,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>32</v>
+      </c>
+      <c r="F90" s="13">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="G90" s="13">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>112</v>
+      </c>
+      <c r="B91" t="s">
+        <v>113</v>
+      </c>
+      <c r="C91" s="3">
+        <v>2</v>
+      </c>
+      <c r="D91" s="3">
+        <f>VLOOKUP(C91,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>8</v>
+      </c>
+      <c r="F91" s="13">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="G91" s="13">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>112</v>
+      </c>
+      <c r="B92" t="s">
+        <v>114</v>
+      </c>
+      <c r="C92" s="3">
+        <v>2</v>
+      </c>
+      <c r="D92" s="3">
+        <f>VLOOKUP(C92,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>8</v>
+      </c>
+      <c r="F92" s="13">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="G92" s="13">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>112</v>
+      </c>
+      <c r="B93" t="s">
+        <v>115</v>
+      </c>
+      <c r="C93" s="3">
+        <v>5</v>
+      </c>
+      <c r="D93" s="3">
+        <f>VLOOKUP(C93,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>32</v>
+      </c>
+      <c r="F93" s="13">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="G93" s="13">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>112</v>
+      </c>
+      <c r="B94" t="s">
+        <v>116</v>
+      </c>
+      <c r="C94" s="3">
+        <v>5</v>
+      </c>
+      <c r="D94" s="3">
+        <f>VLOOKUP(C94,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>32</v>
+      </c>
+      <c r="F94" s="13">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="G94" s="13">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>112</v>
+      </c>
+      <c r="B95" t="s">
+        <v>117</v>
+      </c>
+      <c r="C95" s="3">
+        <v>5</v>
+      </c>
+      <c r="D95" s="3">
+        <f>VLOOKUP(C95,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>32</v>
+      </c>
+      <c r="F95" s="13">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="G95" s="13">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>136</v>
+      </c>
+      <c r="B96" t="s">
+        <v>137</v>
+      </c>
+      <c r="C96" s="3">
+        <v>2</v>
+      </c>
+      <c r="D96" s="3">
+        <f>VLOOKUP(C96,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>8</v>
+      </c>
+      <c r="F96">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="G96">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A98" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="B98" s="4"/>
+      <c r="C98" s="5">
+        <f>SUM(C2:C97)</f>
+        <v>274</v>
+      </c>
+      <c r="D98" s="5">
+        <f>SUM(D2:D97)</f>
+        <v>1484</v>
+      </c>
+      <c r="F98" s="4">
+        <f>SUM(F2:F97)</f>
+        <v>32</v>
+      </c>
+      <c r="G98">
+        <f>SUM(G2:G97)</f>
+        <v>136</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A99" s="6"/>
+      <c r="B99" s="4"/>
+      <c r="C99" s="5"/>
+      <c r="D99" s="5"/>
+      <c r="G99" s="4"/>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A100" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="B100" s="11">
+        <f>D98/Resources!B7</f>
+        <v>31.574468085106382</v>
+      </c>
+      <c r="D100" s="7"/>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A101" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="B101" s="11">
+        <f ca="1">(D98-G98)/B106</f>
+        <v>79.294117647058826</v>
+      </c>
+      <c r="D101" s="7"/>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A102" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="B102" s="4">
+        <f ca="1">FLOOR(((TODAY()-Variables!B2)/7),1)</f>
+        <v>8</v>
+      </c>
+      <c r="D102" s="7"/>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A103" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="B89" t="s">
-        <v>141</v>
-      </c>
-      <c r="C89" s="3">
-        <v>2</v>
-      </c>
-      <c r="D89" s="3">
-        <f>VLOOKUP(Table1[[#This Row],[Points]],Points!$A$1:$C$6,3,FALSE)</f>
-        <v>8</v>
-      </c>
-      <c r="F89">
-        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
-      </c>
-      <c r="G89">
-        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A91" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="B91" s="4"/>
-      <c r="C91" s="5">
-        <f>SUM(C2:C90)</f>
-        <v>243</v>
-      </c>
-      <c r="D91" s="5">
-        <f>SUM(D2:D90)</f>
-        <v>1296</v>
-      </c>
-      <c r="F91" s="4">
-        <f>SUM(F2:F90)</f>
-        <v>24</v>
-      </c>
-      <c r="G91">
-        <f>SUM(G2:G90)</f>
-        <v>96</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A92" s="6"/>
-      <c r="B92" s="4"/>
-      <c r="C92" s="5"/>
-      <c r="D92" s="5"/>
-      <c r="G92" s="4"/>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A93" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="B93" s="11">
-        <f>D91/Resources!B6</f>
-        <v>108</v>
-      </c>
-      <c r="D93" s="7"/>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A94" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="B94" s="11">
-        <f ca="1">(D91-G91)/B99</f>
-        <v>75</v>
-      </c>
-      <c r="D94" s="7"/>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A95" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="B95" s="4">
-        <f ca="1">FLOOR(((TODAY()-Variables!B2)/7),1)</f>
-        <v>6</v>
-      </c>
-      <c r="D95" s="7"/>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A96" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="B96" s="12">
+      <c r="B103" s="12">
         <f>Variables!B2</f>
         <v>44892</v>
       </c>
-      <c r="D96" s="7"/>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A97" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="B97" s="12">
-        <f ca="1">TODAY()+ (B94*7)</f>
-        <v>45459</v>
-      </c>
-      <c r="D97" s="9"/>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A98" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="B98" s="11">
-        <f ca="1">F91/B95</f>
-        <v>4</v>
-      </c>
-      <c r="F98" s="10"/>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A99" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="B99" s="4">
-        <f ca="1">G91/B95</f>
-        <v>16</v>
+      <c r="D103" s="7"/>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A104" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="B104" s="12">
+        <f ca="1">TODAY()+ (B101*7)</f>
+        <v>45504.058823529413</v>
+      </c>
+      <c r="D104" s="9"/>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A105" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="B105" s="11">
+        <f ca="1">F98/B102</f>
+        <v>4</v>
+      </c>
+      <c r="F105" s="10"/>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A106" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="B106" s="4">
+        <f ca="1">G98/B102</f>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -3160,10 +3329,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{686172D1-3F7C-4409-81BD-9F9C60450429}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3191,146 +3360,34 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F1" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="G1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>109</v>
-      </c>
-      <c r="B2" t="s">
-        <v>108</v>
-      </c>
       <c r="C2" s="3">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D2" s="3">
-        <f>VLOOKUP(C2,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>109</v>
-      </c>
-      <c r="B3" t="s">
-        <v>110</v>
-      </c>
-      <c r="C3" s="3">
-        <v>3</v>
-      </c>
-      <c r="D3" s="3">
-        <f>VLOOKUP(C3,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>109</v>
-      </c>
-      <c r="B4" t="s">
-        <v>111</v>
-      </c>
-      <c r="C4" s="3">
-        <v>5</v>
-      </c>
-      <c r="D4" s="3">
-        <f>VLOOKUP(C4,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>112</v>
-      </c>
-      <c r="B5" t="s">
-        <v>113</v>
-      </c>
-      <c r="C5" s="3">
-        <v>2</v>
-      </c>
-      <c r="D5" s="3">
-        <f>VLOOKUP(C5,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>112</v>
-      </c>
-      <c r="B6" t="s">
-        <v>114</v>
-      </c>
-      <c r="C6" s="3">
-        <v>2</v>
-      </c>
-      <c r="D6" s="3">
-        <f>VLOOKUP(C6,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>112</v>
-      </c>
-      <c r="B7" t="s">
-        <v>115</v>
-      </c>
-      <c r="C7" s="3">
-        <v>5</v>
-      </c>
-      <c r="D7" s="3">
-        <f>VLOOKUP(C7,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>112</v>
-      </c>
-      <c r="B8" t="s">
-        <v>116</v>
-      </c>
-      <c r="C8" s="3">
-        <v>5</v>
-      </c>
-      <c r="D8" s="3">
-        <f>VLOOKUP(C8,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>112</v>
-      </c>
-      <c r="B9" t="s">
-        <v>117</v>
-      </c>
-      <c r="C9" s="3">
-        <v>5</v>
-      </c>
-      <c r="D9" s="3">
-        <f>VLOOKUP(C9,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>142</v>
-      </c>
-      <c r="C11">
-        <f>SUM(C2:C10)</f>
-        <v>32</v>
-      </c>
-      <c r="D11">
-        <f>SUM(D2:D10)</f>
-        <v>192</v>
+        <v>138</v>
+      </c>
+      <c r="C4">
+        <f>SUM(C2:C3)</f>
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <f>SUM(D2:D3)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3429,14 +3486,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F621DB0-8DAE-49A3-A9ED-9FDE92100FD7}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="38.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3445,12 +3503,12 @@
         <v>119</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>120</v>
+        <v>141</v>
       </c>
       <c r="B2">
         <v>8</v>
@@ -3458,7 +3516,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>121</v>
+        <v>142</v>
       </c>
       <c r="B3">
         <v>4</v>
@@ -3466,19 +3524,27 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>126</v>
+        <v>143</v>
       </c>
       <c r="B4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>144</v>
+      </c>
+      <c r="B5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="B6" s="4">
-        <f>SUM(B2:B4)</f>
-        <v>12</v>
+      <c r="B7" s="4">
+        <f>SUM(B2:B5)</f>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -3501,15 +3567,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B2" s="8">
         <v>44892</v>

</xml_diff>

<commit_message>
Update to project plan and estimates
</commit_message>
<xml_diff>
--- a/Documentation/Design/Estimates.xlsx
+++ b/Documentation/Design/Estimates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_git\BedBrigadeNational\Documentation\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC610649-9682-4E2D-A867-35E48510554D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEE41FA5-BBFF-4C1C-B037-5FE608016CDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D27F5AFA-C88C-4A2F-A896-BFED2572A1C7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D27F5AFA-C88C-4A2F-A896-BFED2572A1C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Estimates" sheetId="1" r:id="rId1"/>
@@ -531,7 +531,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -557,16 +557,11 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="6">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -579,6 +574,10 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -603,14 +602,14 @@
     <tableColumn id="2" xr3:uid="{8122BCC0-A9A0-4E8A-97F8-809454E87965}" name="Epic"/>
     <tableColumn id="3" xr3:uid="{62273C57-4035-404E-BD7F-DBE541848AF0}" name="Story"/>
     <tableColumn id="4" xr3:uid="{F83CC626-5103-462B-9E71-70FF58ECD672}" name="Points" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{32A1D275-1575-4B11-A22D-5A36CD923379}" name="Estimated Hours" dataDxfId="0">
+    <tableColumn id="5" xr3:uid="{32A1D275-1575-4B11-A22D-5A36CD923379}" name="Estimated Hours" dataDxfId="4">
       <calculatedColumnFormula>VLOOKUP(C2,Points!$A$1:$C$6,3,FALSE)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{E075E6CD-1DFD-47F5-B7CE-6A6F43BA85B6}" name="Completed"/>
-    <tableColumn id="8" xr3:uid="{775079EE-6981-4E34-B3C6-3629C5635AE6}" name="Completed Points" dataDxfId="4">
+    <tableColumn id="8" xr3:uid="{775079EE-6981-4E34-B3C6-3629C5635AE6}" name="Completed Points" dataDxfId="3">
       <calculatedColumnFormula>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{B8125C06-D59F-4CA7-817D-1DFF5C288455}" name="Completed Hours" dataDxfId="3">
+    <tableColumn id="7" xr3:uid="{B8125C06-D59F-4CA7-817D-1DFF5C288455}" name="Completed Hours" dataDxfId="2">
       <calculatedColumnFormula>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -624,8 +623,8 @@
   <tableColumns count="7">
     <tableColumn id="2" xr3:uid="{31CB5B43-DDC0-45F7-94FE-8435C1D008DA}" name="Epic"/>
     <tableColumn id="3" xr3:uid="{E8134CEE-EEF4-4605-A21F-CFF015B23BA2}" name="Story"/>
-    <tableColumn id="4" xr3:uid="{A8E050D4-AAEC-4516-ABB3-A0C110009E2F}" name="Points" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{AD6AC57F-E07B-42DB-850E-DEA524AE6E46}" name="Estimated Hours" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{A8E050D4-AAEC-4516-ABB3-A0C110009E2F}" name="Points" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{AD6AC57F-E07B-42DB-850E-DEA524AE6E46}" name="Estimated Hours" dataDxfId="0"/>
     <tableColumn id="6" xr3:uid="{86F5B27A-D198-4848-ADB6-A7BEFFDB816F}" name="Completed"/>
     <tableColumn id="7" xr3:uid="{2398D599-5A1D-4B6E-8A23-79F4063944CE}" name="Completed Points"/>
     <tableColumn id="8" xr3:uid="{C13FCCDE-FC9C-48C6-AE8F-48A44BF6C3D4}" name="Completed Hours"/>
@@ -923,7 +922,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -934,8 +933,8 @@
   <dimension ref="A1:G106"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B106" sqref="B106"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E57" sqref="E57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1552,13 +1551,16 @@
         <f>VLOOKUP(C24,Points!$A$1:$C$6,3,FALSE)</f>
         <v>8</v>
       </c>
+      <c r="E24" t="b">
+        <v>1</v>
+      </c>
       <c r="F24">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G24">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1575,13 +1577,16 @@
         <f>VLOOKUP(C25,Points!$A$1:$C$6,3,FALSE)</f>
         <v>16</v>
       </c>
+      <c r="E25" t="b">
+        <v>1</v>
+      </c>
       <c r="F25">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G25">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1624,13 +1629,16 @@
         <f>VLOOKUP(C27,Points!$A$1:$C$6,3,FALSE)</f>
         <v>16</v>
       </c>
+      <c r="E27" t="b">
+        <v>1</v>
+      </c>
       <c r="F27">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G27">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1647,13 +1655,16 @@
         <f>VLOOKUP(C28,Points!$A$1:$C$6,3,FALSE)</f>
         <v>32</v>
       </c>
+      <c r="E28" t="b">
+        <v>1</v>
+      </c>
       <c r="F28">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G28">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>0</v>
+        <v>32</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -2199,13 +2210,16 @@
         <f>VLOOKUP(C52,Points!$A$1:$C$6,3,FALSE)</f>
         <v>32</v>
       </c>
+      <c r="E52" t="b">
+        <v>1</v>
+      </c>
       <c r="F52">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G52">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>0</v>
+        <v>32</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
@@ -2222,13 +2236,16 @@
         <f>VLOOKUP(C53,Points!$A$1:$C$6,3,FALSE)</f>
         <v>16</v>
       </c>
+      <c r="E53" t="b">
+        <v>1</v>
+      </c>
       <c r="F53">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G53">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
@@ -2245,13 +2262,16 @@
         <f>VLOOKUP(C54,Points!$A$1:$C$6,3,FALSE)</f>
         <v>32</v>
       </c>
+      <c r="E54" t="b">
+        <v>1</v>
+      </c>
       <c r="F54">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G54">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>0</v>
+        <v>32</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
@@ -2314,13 +2334,16 @@
         <f>VLOOKUP(C57,Points!$A$1:$C$6,3,FALSE)</f>
         <v>32</v>
       </c>
+      <c r="E57" t="b">
+        <v>1</v>
+      </c>
       <c r="F57">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G57">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>0</v>
+        <v>32</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
@@ -2429,13 +2452,16 @@
         <f>VLOOKUP(C62,Points!$A$1:$C$6,3,FALSE)</f>
         <v>32</v>
       </c>
+      <c r="E62" t="b">
+        <v>1</v>
+      </c>
       <c r="F62">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G62">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>0</v>
+        <v>32</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
@@ -2636,13 +2662,16 @@
         <f>VLOOKUP(C71,Points!$A$1:$C$6,3,FALSE)</f>
         <v>16</v>
       </c>
+      <c r="E71" t="b">
+        <v>1</v>
+      </c>
       <c r="F71">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G71">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
@@ -2659,13 +2688,16 @@
         <f>VLOOKUP(C72,Points!$A$1:$C$6,3,FALSE)</f>
         <v>16</v>
       </c>
+      <c r="E72" t="b">
+        <v>1</v>
+      </c>
       <c r="F72">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G72">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
@@ -2682,13 +2714,16 @@
         <f>VLOOKUP(C73,Points!$A$1:$C$6,3,FALSE)</f>
         <v>16</v>
       </c>
+      <c r="E73" t="b">
+        <v>1</v>
+      </c>
       <c r="F73">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G73">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
@@ -2705,13 +2740,16 @@
         <f>VLOOKUP(C74,Points!$A$1:$C$6,3,FALSE)</f>
         <v>16</v>
       </c>
+      <c r="E74" t="b">
+        <v>1</v>
+      </c>
       <c r="F74">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G74">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
@@ -3027,11 +3065,11 @@
         <f>VLOOKUP(C88,Points!$A$1:$C$6,3,FALSE)</f>
         <v>32</v>
       </c>
-      <c r="F88" s="13">
-        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
-      </c>
-      <c r="G88" s="13">
+      <c r="F88">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="G88">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
         <v>0</v>
       </c>
@@ -3050,11 +3088,11 @@
         <f>VLOOKUP(C89,Points!$A$1:$C$6,3,FALSE)</f>
         <v>16</v>
       </c>
-      <c r="F89" s="13">
-        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
-      </c>
-      <c r="G89" s="13">
+      <c r="F89">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="G89">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
         <v>0</v>
       </c>
@@ -3073,11 +3111,11 @@
         <f>VLOOKUP(C90,Points!$A$1:$C$6,3,FALSE)</f>
         <v>32</v>
       </c>
-      <c r="F90" s="13">
-        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
-      </c>
-      <c r="G90" s="13">
+      <c r="F90">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="G90">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
         <v>0</v>
       </c>
@@ -3096,11 +3134,11 @@
         <f>VLOOKUP(C91,Points!$A$1:$C$6,3,FALSE)</f>
         <v>8</v>
       </c>
-      <c r="F91" s="13">
-        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
-      </c>
-      <c r="G91" s="13">
+      <c r="F91">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="G91">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
         <v>0</v>
       </c>
@@ -3119,11 +3157,11 @@
         <f>VLOOKUP(C92,Points!$A$1:$C$6,3,FALSE)</f>
         <v>8</v>
       </c>
-      <c r="F92" s="13">
-        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
-      </c>
-      <c r="G92" s="13">
+      <c r="F92">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="G92">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
         <v>0</v>
       </c>
@@ -3142,11 +3180,11 @@
         <f>VLOOKUP(C93,Points!$A$1:$C$6,3,FALSE)</f>
         <v>32</v>
       </c>
-      <c r="F93" s="13">
-        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
-      </c>
-      <c r="G93" s="13">
+      <c r="F93">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="G93">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
         <v>0</v>
       </c>
@@ -3165,11 +3203,11 @@
         <f>VLOOKUP(C94,Points!$A$1:$C$6,3,FALSE)</f>
         <v>32</v>
       </c>
-      <c r="F94" s="13">
-        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
-      </c>
-      <c r="G94" s="13">
+      <c r="F94">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="G94">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
         <v>0</v>
       </c>
@@ -3188,11 +3226,11 @@
         <f>VLOOKUP(C95,Points!$A$1:$C$6,3,FALSE)</f>
         <v>32</v>
       </c>
-      <c r="F95" s="13">
-        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
-      </c>
-      <c r="G95" s="13">
+      <c r="F95">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="G95">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
         <v>0</v>
       </c>
@@ -3235,11 +3273,11 @@
       </c>
       <c r="F98" s="4">
         <f>SUM(F2:F97)</f>
-        <v>32</v>
+        <v>80</v>
       </c>
       <c r="G98">
         <f>SUM(G2:G97)</f>
-        <v>136</v>
+        <v>416</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
@@ -3265,7 +3303,7 @@
       </c>
       <c r="B101" s="11">
         <f ca="1">(D98-G98)/B106</f>
-        <v>79.294117647058826</v>
+        <v>33.375</v>
       </c>
       <c r="D101" s="7"/>
     </row>
@@ -3275,7 +3313,7 @@
       </c>
       <c r="B102" s="4">
         <f ca="1">FLOOR(((TODAY()-Variables!B2)/7),1)</f>
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D102" s="7"/>
     </row>
@@ -3295,7 +3333,7 @@
       </c>
       <c r="B104" s="12">
         <f ca="1">TODAY()+ (B101*7)</f>
-        <v>45504.058823529413</v>
+        <v>45222.625</v>
       </c>
       <c r="D104" s="9"/>
     </row>
@@ -3305,7 +3343,7 @@
       </c>
       <c r="B105" s="11">
         <f ca="1">F98/B102</f>
-        <v>4</v>
+        <v>6.1538461538461542</v>
       </c>
       <c r="F105" s="10"/>
     </row>
@@ -3315,7 +3353,7 @@
       </c>
       <c r="B106" s="4">
         <f ca="1">G98/B102</f>
-        <v>17</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix for infinite loop for donations.  Update estimates and Project Plan.
</commit_message>
<xml_diff>
--- a/Documentation/Design/Estimates.xlsx
+++ b/Documentation/Design/Estimates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_git\BedBrigadeNational\Documentation\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E16E4FE3-5A76-40E7-8101-BA78217C9378}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9BD0D84-D6B1-433D-BE1E-8260E35BBD26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D27F5AFA-C88C-4A2F-A896-BFED2572A1C7}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="146">
   <si>
     <t>Epic</t>
   </si>
@@ -475,6 +475,9 @@
   </si>
   <si>
     <t>Val Skordin</t>
+  </si>
+  <si>
+    <t>Manage Build and Delivery Schedule</t>
   </si>
 </sst>
 </file>
@@ -531,7 +534,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -557,6 +560,10 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -596,8 +603,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{20A5C34A-BA74-4618-9527-C8C5A4B15239}" name="Table1" displayName="Table1" ref="A1:G96" totalsRowShown="0">
-  <autoFilter ref="A1:G96" xr:uid="{20A5C34A-BA74-4618-9527-C8C5A4B15239}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{20A5C34A-BA74-4618-9527-C8C5A4B15239}" name="Table1" displayName="Table1" ref="A1:G97" totalsRowShown="0">
+  <autoFilter ref="A1:G97" xr:uid="{20A5C34A-BA74-4618-9527-C8C5A4B15239}"/>
   <tableColumns count="7">
     <tableColumn id="2" xr3:uid="{8122BCC0-A9A0-4E8A-97F8-809454E87965}" name="Epic"/>
     <tableColumn id="3" xr3:uid="{62273C57-4035-404E-BD7F-DBE541848AF0}" name="Story"/>
@@ -930,11 +937,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F9D3302-E5F0-4E5C-9EB3-B74DDF37DF9D}">
-  <dimension ref="A1:G106"/>
+  <dimension ref="A1:G107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B104" sqref="B104"/>
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2522,23 +2529,23 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B64" t="s">
-        <v>80</v>
+        <v>145</v>
       </c>
       <c r="C64" s="3">
-        <v>3</v>
-      </c>
-      <c r="D64" s="3">
+        <v>5</v>
+      </c>
+      <c r="D64" s="13">
         <f>VLOOKUP(C64,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>16</v>
-      </c>
-      <c r="F64">
-        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
-      </c>
-      <c r="G64">
+        <v>32</v>
+      </c>
+      <c r="F64" s="14">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="G64" s="14">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
         <v>0</v>
       </c>
@@ -2548,14 +2555,14 @@
         <v>79</v>
       </c>
       <c r="B65" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C65" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D65" s="3">
         <f>VLOOKUP(C65,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="F65">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
@@ -2568,10 +2575,10 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B66" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C66" s="3">
         <v>5</v>
@@ -2594,14 +2601,14 @@
         <v>82</v>
       </c>
       <c r="B67" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C67" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D67" s="3">
         <f>VLOOKUP(C67,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="F67">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
@@ -2617,7 +2624,7 @@
         <v>82</v>
       </c>
       <c r="B68" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C68" s="3">
         <v>3</v>
@@ -2640,14 +2647,14 @@
         <v>82</v>
       </c>
       <c r="B69" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C69" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D69" s="3">
         <f>VLOOKUP(C69,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="F69">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
@@ -2663,7 +2670,7 @@
         <v>82</v>
       </c>
       <c r="B70" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C70" s="3">
         <v>5</v>
@@ -2683,28 +2690,25 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B71" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C71" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D71" s="3">
         <f>VLOOKUP(C71,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>16</v>
-      </c>
-      <c r="E71" t="b">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="F71">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G71">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
@@ -2712,7 +2716,7 @@
         <v>88</v>
       </c>
       <c r="B72" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C72" s="3">
         <v>3</v>
@@ -2738,7 +2742,7 @@
         <v>88</v>
       </c>
       <c r="B73" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C73" s="3">
         <v>3</v>
@@ -2747,13 +2751,16 @@
         <f>VLOOKUP(C73,Points!$A$1:$C$6,3,FALSE)</f>
         <v>16</v>
       </c>
+      <c r="E73" t="b">
+        <v>1</v>
+      </c>
       <c r="F73">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G73">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
@@ -2761,7 +2768,7 @@
         <v>88</v>
       </c>
       <c r="B74" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C74" s="3">
         <v>3</v>
@@ -2770,24 +2777,21 @@
         <f>VLOOKUP(C74,Points!$A$1:$C$6,3,FALSE)</f>
         <v>16</v>
       </c>
-      <c r="E74" t="b">
-        <v>1</v>
-      </c>
       <c r="F74">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G74">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B75" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C75" s="3">
         <v>3</v>
@@ -2796,13 +2800,16 @@
         <f>VLOOKUP(C75,Points!$A$1:$C$6,3,FALSE)</f>
         <v>16</v>
       </c>
+      <c r="E75" t="b">
+        <v>1</v>
+      </c>
       <c r="F75">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G75">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
@@ -2810,7 +2817,7 @@
         <v>93</v>
       </c>
       <c r="B76" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C76" s="3">
         <v>3</v>
@@ -2833,7 +2840,7 @@
         <v>93</v>
       </c>
       <c r="B77" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C77" s="3">
         <v>3</v>
@@ -2856,7 +2863,7 @@
         <v>93</v>
       </c>
       <c r="B78" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C78" s="3">
         <v>3</v>
@@ -2879,7 +2886,7 @@
         <v>93</v>
       </c>
       <c r="B79" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C79" s="3">
         <v>3</v>
@@ -2902,14 +2909,14 @@
         <v>93</v>
       </c>
       <c r="B80" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C80" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D80" s="3">
         <f>VLOOKUP(C80,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="F80">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
@@ -2922,10 +2929,10 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="B81" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C81" s="3">
         <v>2</v>
@@ -2948,7 +2955,7 @@
         <v>100</v>
       </c>
       <c r="B82" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C82" s="3">
         <v>2</v>
@@ -2971,7 +2978,7 @@
         <v>100</v>
       </c>
       <c r="B83" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C83" s="3">
         <v>2</v>
@@ -2994,7 +3001,7 @@
         <v>100</v>
       </c>
       <c r="B84" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C84" s="3">
         <v>2</v>
@@ -3017,7 +3024,7 @@
         <v>100</v>
       </c>
       <c r="B85" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C85" s="3">
         <v>2</v>
@@ -3040,7 +3047,7 @@
         <v>100</v>
       </c>
       <c r="B86" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C86" s="3">
         <v>2</v>
@@ -3063,7 +3070,7 @@
         <v>100</v>
       </c>
       <c r="B87" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C87" s="3">
         <v>2</v>
@@ -3083,17 +3090,17 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B88" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C88" s="3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D88" s="3">
         <f>VLOOKUP(C88,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="F88">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
@@ -3109,14 +3116,14 @@
         <v>109</v>
       </c>
       <c r="B89" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C89" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D89" s="3">
         <f>VLOOKUP(C89,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="F89">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
@@ -3132,14 +3139,14 @@
         <v>109</v>
       </c>
       <c r="B90" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C90" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D90" s="3">
         <f>VLOOKUP(C90,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="F90">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
@@ -3152,17 +3159,17 @@
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B91" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C91" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D91" s="3">
         <f>VLOOKUP(C91,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="F91">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
@@ -3178,7 +3185,7 @@
         <v>112</v>
       </c>
       <c r="B92" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C92" s="3">
         <v>2</v>
@@ -3201,14 +3208,14 @@
         <v>112</v>
       </c>
       <c r="B93" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C93" s="3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D93" s="3">
         <f>VLOOKUP(C93,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="F93">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
@@ -3224,7 +3231,7 @@
         <v>112</v>
       </c>
       <c r="B94" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C94" s="3">
         <v>5</v>
@@ -3247,7 +3254,7 @@
         <v>112</v>
       </c>
       <c r="B95" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C95" s="3">
         <v>5</v>
@@ -3267,17 +3274,17 @@
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>136</v>
+        <v>112</v>
       </c>
       <c r="B96" t="s">
-        <v>137</v>
+        <v>117</v>
       </c>
       <c r="C96" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D96" s="3">
         <f>VLOOKUP(C96,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="F96">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
@@ -3288,102 +3295,125 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A98" s="6" t="s">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>136</v>
+      </c>
+      <c r="B97" t="s">
+        <v>137</v>
+      </c>
+      <c r="C97" s="3">
+        <v>2</v>
+      </c>
+      <c r="D97" s="3">
+        <f>VLOOKUP(C97,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>8</v>
+      </c>
+      <c r="F97">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="G97">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A99" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="B98" s="4"/>
-      <c r="C98" s="5">
-        <f>SUM(C2:C97)</f>
-        <v>274</v>
-      </c>
-      <c r="D98" s="5">
-        <f>SUM(D2:D97)</f>
-        <v>1484</v>
-      </c>
-      <c r="F98" s="4">
-        <f>SUM(F2:F97)</f>
+      <c r="B99" s="4"/>
+      <c r="C99" s="5">
+        <f>SUM(C2:C98)</f>
+        <v>279</v>
+      </c>
+      <c r="D99" s="5">
+        <f>SUM(D2:D98)</f>
+        <v>1516</v>
+      </c>
+      <c r="F99" s="4">
+        <f>SUM(F2:F98)</f>
         <v>104</v>
       </c>
-      <c r="G98">
-        <f>SUM(G2:G97)</f>
+      <c r="G99">
+        <f>SUM(G2:G98)</f>
         <v>532</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A99" s="6"/>
-      <c r="B99" s="4"/>
-      <c r="C99" s="5"/>
-      <c r="D99" s="5"/>
-      <c r="G99" s="4"/>
-    </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A100" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="B100" s="11">
-        <f>D98/Resources!B7</f>
-        <v>31.574468085106382</v>
-      </c>
-      <c r="D100" s="7"/>
+      <c r="A100" s="6"/>
+      <c r="B100" s="4"/>
+      <c r="C100" s="5"/>
+      <c r="D100" s="5"/>
+      <c r="G100" s="4"/>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="6" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="B101" s="11">
-        <f ca="1">(D98-G98)/B106</f>
-        <v>39.368421052631575</v>
+        <f>D99/Resources!B7</f>
+        <v>32.255319148936174</v>
       </c>
       <c r="D101" s="7"/>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="B102" s="4">
-        <f ca="1">FLOOR(((TODAY()-Variables!B2)/7),1)</f>
-        <v>22</v>
+        <v>139</v>
+      </c>
+      <c r="B102" s="11">
+        <f ca="1">(D99-G99)/B107</f>
+        <v>42.541353383458649</v>
       </c>
       <c r="D102" s="7"/>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="B103" s="4">
+        <f ca="1">FLOOR(((TODAY()-Variables!B2)/7),1)</f>
+        <v>23</v>
+      </c>
+      <c r="D103" s="7"/>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A104" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="B103" s="12">
+      <c r="B104" s="12">
         <f>Variables!B2</f>
         <v>44892</v>
       </c>
-      <c r="D103" s="7"/>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A104" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="B104" s="12">
-        <f ca="1">TODAY()+ (B101*7)</f>
-        <v>45327.57894736842</v>
-      </c>
-      <c r="D104" s="9"/>
+      <c r="D104" s="7"/>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="B105" s="11">
-        <f ca="1">F98/B102</f>
-        <v>4.7272727272727275</v>
-      </c>
-      <c r="F105" s="10"/>
+        <v>127</v>
+      </c>
+      <c r="B105" s="12">
+        <f ca="1">TODAY()+ (B102*7)</f>
+        <v>45352.789473684214</v>
+      </c>
+      <c r="D105" s="9"/>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="B106" s="11">
+        <f ca="1">F99/B103</f>
+        <v>4.5217391304347823</v>
+      </c>
+      <c r="F106" s="10"/>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A107" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="B106" s="4">
-        <f ca="1">G98/B102</f>
-        <v>24.181818181818183</v>
+      <c r="B107" s="4">
+        <f ca="1">G99/B103</f>
+        <v>23.130434782608695</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update estimates and project plan
</commit_message>
<xml_diff>
--- a/Documentation/Design/Estimates.xlsx
+++ b/Documentation/Design/Estimates.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_git\BedBrigadeNational\Documentation\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6155A3B-95D2-4E34-86C1-8338B5104BBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C10D4EF7-E310-4F4C-BCBD-7E166A7270ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D27F5AFA-C88C-4A2F-A896-BFED2572A1C7}"/>
   </bookViews>
@@ -940,7 +940,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B100" sqref="B100"/>
+      <selection pane="bottomLeft" activeCell="E65" sqref="E65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1693,13 +1693,16 @@
         <f>VLOOKUP(C29,Points!$A$1:$C$6,3,FALSE)</f>
         <v>32</v>
       </c>
+      <c r="E29" t="b">
+        <v>1</v>
+      </c>
       <c r="F29">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G29">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>0</v>
+        <v>32</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -1950,13 +1953,16 @@
         <f>VLOOKUP(C39,Points!$A$1:$C$6,3,FALSE)</f>
         <v>32</v>
       </c>
+      <c r="E39" t="b">
+        <v>1</v>
+      </c>
       <c r="F39">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G39">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>0</v>
+        <v>32</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -1973,13 +1979,16 @@
         <f>VLOOKUP(C40,Points!$A$1:$C$6,3,FALSE)</f>
         <v>8</v>
       </c>
+      <c r="E40" t="b">
+        <v>1</v>
+      </c>
       <c r="F40">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G40">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -1996,13 +2005,16 @@
         <f>VLOOKUP(C41,Points!$A$1:$C$6,3,FALSE)</f>
         <v>8</v>
       </c>
+      <c r="E41" t="b">
+        <v>1</v>
+      </c>
       <c r="F41">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G41">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -2019,13 +2031,16 @@
         <f>VLOOKUP(C42,Points!$A$1:$C$6,3,FALSE)</f>
         <v>8</v>
       </c>
+      <c r="E42" t="b">
+        <v>1</v>
+      </c>
       <c r="F42">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G42">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -2552,13 +2567,16 @@
         <f>VLOOKUP(C64,Points!$A$1:$C$6,3,FALSE)</f>
         <v>32</v>
       </c>
+      <c r="E64" t="b">
+        <v>1</v>
+      </c>
       <c r="F64">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G64">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>0</v>
+        <v>32</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
@@ -3186,11 +3204,11 @@
       </c>
       <c r="F92" s="4">
         <f>SUM(F2:F91)</f>
-        <v>124</v>
+        <v>145</v>
       </c>
       <c r="G92">
         <f>SUM(G2:G91)</f>
-        <v>652</v>
+        <v>772</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
@@ -3206,7 +3224,7 @@
       </c>
       <c r="B94" s="11">
         <f ca="1">B96+B95</f>
-        <v>61.656441717791409</v>
+        <v>62.487046632124354</v>
       </c>
       <c r="D94" s="7"/>
     </row>
@@ -3216,7 +3234,7 @@
       </c>
       <c r="B95" s="11">
         <f ca="1">(D92-G92)/B100</f>
-        <v>31.656441717791409</v>
+        <v>26.487046632124354</v>
       </c>
       <c r="D95" s="7"/>
     </row>
@@ -3226,7 +3244,7 @@
       </c>
       <c r="B96" s="4">
         <f ca="1">FLOOR(((TODAY()-Variables!B2)/7),1)</f>
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="D96" s="7"/>
     </row>
@@ -3246,7 +3264,7 @@
       </c>
       <c r="B98" s="12">
         <f ca="1">TODAY()+ (B95*7)</f>
-        <v>45329.595092024538</v>
+        <v>45329.409326424873</v>
       </c>
       <c r="D98" s="9"/>
     </row>
@@ -3256,7 +3274,7 @@
       </c>
       <c r="B99" s="11">
         <f ca="1">F92/B96</f>
-        <v>4.1333333333333337</v>
+        <v>4.0277777777777777</v>
       </c>
       <c r="F99" s="10"/>
     </row>
@@ -3266,7 +3284,7 @@
       </c>
       <c r="B100" s="4">
         <f ca="1">G92/B96</f>
-        <v>21.733333333333334</v>
+        <v>21.444444444444443</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Project Plan.md and Estimates.xlsx. Add titles to BedRequestForm.razor and ContactUsForm.razor
</commit_message>
<xml_diff>
--- a/Documentation/Design/Estimates.xlsx
+++ b/Documentation/Design/Estimates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_git\BedBrigadeNational\Documentation\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C10D4EF7-E310-4F4C-BCBD-7E166A7270ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94392AB6-B431-4D31-AB92-7D17C230FB69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D27F5AFA-C88C-4A2F-A896-BFED2572A1C7}"/>
   </bookViews>
@@ -939,8 +939,8 @@
   <dimension ref="A1:G100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E65" sqref="E65"/>
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E67" sqref="E67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2377,13 +2377,16 @@
         <f>VLOOKUP(C56,Points!$A$1:$C$6,3,FALSE)</f>
         <v>32</v>
       </c>
+      <c r="E56" t="b">
+        <v>1</v>
+      </c>
       <c r="F56">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G56">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>0</v>
+        <v>32</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
@@ -2593,13 +2596,16 @@
         <f>VLOOKUP(C65,Points!$A$1:$C$6,3,FALSE)</f>
         <v>16</v>
       </c>
+      <c r="E65" t="b">
+        <v>1</v>
+      </c>
       <c r="F65">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G65">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
@@ -2616,13 +2622,16 @@
         <f>VLOOKUP(C66,Points!$A$1:$C$6,3,FALSE)</f>
         <v>32</v>
       </c>
+      <c r="E66" t="b">
+        <v>1</v>
+      </c>
       <c r="F66">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G66">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>0</v>
+        <v>32</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
@@ -3204,11 +3213,11 @@
       </c>
       <c r="F92" s="4">
         <f>SUM(F2:F91)</f>
-        <v>145</v>
+        <v>158</v>
       </c>
       <c r="G92">
         <f>SUM(G2:G91)</f>
-        <v>772</v>
+        <v>852</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
@@ -3224,7 +3233,7 @@
       </c>
       <c r="B94" s="11">
         <f ca="1">B96+B95</f>
-        <v>62.487046632124354</v>
+        <v>61.338028169014081</v>
       </c>
       <c r="D94" s="7"/>
     </row>
@@ -3234,7 +3243,7 @@
       </c>
       <c r="B95" s="11">
         <f ca="1">(D92-G92)/B100</f>
-        <v>26.487046632124354</v>
+        <v>22.338028169014084</v>
       </c>
       <c r="D95" s="7"/>
     </row>
@@ -3244,7 +3253,7 @@
       </c>
       <c r="B96" s="4">
         <f ca="1">FLOOR(((TODAY()-Variables!B2)/7),1)</f>
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D96" s="7"/>
     </row>
@@ -3264,7 +3273,7 @@
       </c>
       <c r="B98" s="12">
         <f ca="1">TODAY()+ (B95*7)</f>
-        <v>45329.409326424873</v>
+        <v>45324.366197183095</v>
       </c>
       <c r="D98" s="9"/>
     </row>
@@ -3274,7 +3283,7 @@
       </c>
       <c r="B99" s="11">
         <f ca="1">F92/B96</f>
-        <v>4.0277777777777777</v>
+        <v>4.0512820512820511</v>
       </c>
       <c r="F99" s="10"/>
     </row>
@@ -3284,7 +3293,7 @@
       </c>
       <c r="B100" s="4">
         <f ca="1">G92/B96</f>
-        <v>21.444444444444443</v>
+        <v>21.846153846153847</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Project Plan, Estimates, and add Story Points.md
</commit_message>
<xml_diff>
--- a/Documentation/Design/Estimates.xlsx
+++ b/Documentation/Design/Estimates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_git\BedBrigadeNational\Documentation\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC31C618-B9F2-46F1-8C1F-5E56308AEE3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A9171BC-3501-4C0C-99E9-CF894D9F5CDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D27F5AFA-C88C-4A2F-A896-BFED2572A1C7}"/>
+    <workbookView xWindow="-24098" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{D27F5AFA-C88C-4A2F-A896-BFED2572A1C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Estimates" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="183">
   <si>
     <t>Epic</t>
   </si>
@@ -261,9 +261,6 @@
     <t>Schedule Deliveries</t>
   </si>
   <si>
-    <t>Delivery Checklist</t>
-  </si>
-  <si>
     <t>Bulk Email Scheduled Deliveries</t>
   </si>
   <si>
@@ -414,9 +411,6 @@
     <t>Start Date</t>
   </si>
   <si>
-    <t>Week Number</t>
-  </si>
-  <si>
     <t>Estimated Completion Date</t>
   </si>
   <si>
@@ -475,6 +469,126 @@
   </si>
   <si>
     <t>Manage Stories</t>
+  </si>
+  <si>
+    <t>Elapsed Weeks</t>
+  </si>
+  <si>
+    <t>Project Delay in Weeks</t>
+  </si>
+  <si>
+    <t>Project Week Number Accounting for Delay</t>
+  </si>
+  <si>
+    <t>Design National Home Page</t>
+  </si>
+  <si>
+    <t>National Home Page</t>
+  </si>
+  <si>
+    <t>Grove City Location About Us Page</t>
+  </si>
+  <si>
+    <t>Grove City History Page</t>
+  </si>
+  <si>
+    <t>Polaris About Us Page</t>
+  </si>
+  <si>
+    <t>Manage Delivery Checklist</t>
+  </si>
+  <si>
+    <t>Scheduled Deliveries Email Checklist</t>
+  </si>
+  <si>
+    <t>Tech Debt</t>
+  </si>
+  <si>
+    <t>Upgrade to Blazor 8</t>
+  </si>
+  <si>
+    <t>Refactor Common.cs</t>
+  </si>
+  <si>
+    <t>Refactor into Files</t>
+  </si>
+  <si>
+    <t>Move Entities</t>
+  </si>
+  <si>
+    <t>Move Syncfusion Licensing</t>
+  </si>
+  <si>
+    <t>Regression Testing</t>
+  </si>
+  <si>
+    <t>Change from Azure Email to SmarterASP.NET Email</t>
+  </si>
+  <si>
+    <t>Update Diagrams</t>
+  </si>
+  <si>
+    <t>GitHub Actions for Pull Requests</t>
+  </si>
+  <si>
+    <t>Deploy to SmarterASP.NET Development</t>
+  </si>
+  <si>
+    <t>Use location query parm Bed Request</t>
+  </si>
+  <si>
+    <t>Use Location Query Parm Contact</t>
+  </si>
+  <si>
+    <t>Use Location Query Parm Volunteer</t>
+  </si>
+  <si>
+    <t>Design Shared Bed Requests</t>
+  </si>
+  <si>
+    <t>Admin Dashboard Content</t>
+  </si>
+  <si>
+    <t>Unique Volunteer Email Add Dialog</t>
+  </si>
+  <si>
+    <t>Update NuGet Packages and Change NUnit Assertions</t>
+  </si>
+  <si>
+    <t>Cache get files</t>
+  </si>
+  <si>
+    <t>Remove Unused Components and Pages</t>
+  </si>
+  <si>
+    <t>Add three image rotators to Bed Brigade Near Me</t>
+  </si>
+  <si>
+    <t>Location Latitude &amp; Longitude</t>
+  </si>
+  <si>
+    <t>FM Dependent Functionality</t>
+  </si>
+  <si>
+    <t>Verify security for all pages</t>
+  </si>
+  <si>
+    <t>Global Error Handler</t>
+  </si>
+  <si>
+    <t>Refresh Header and Footer</t>
+  </si>
+  <si>
+    <t>Minify CSS and JS</t>
+  </si>
+  <si>
+    <t>Add Page Titles</t>
+  </si>
+  <si>
+    <t>Custom Icons in Grid Toolbar</t>
+  </si>
+  <si>
+    <t>Review All Code</t>
   </si>
 </sst>
 </file>
@@ -531,7 +645,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -557,6 +671,11 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -564,16 +683,16 @@
   <dxfs count="6">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -596,20 +715,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{20A5C34A-BA74-4618-9527-C8C5A4B15239}" name="Table1" displayName="Table1" ref="A1:G90" totalsRowShown="0">
-  <autoFilter ref="A1:G90" xr:uid="{20A5C34A-BA74-4618-9527-C8C5A4B15239}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{20A5C34A-BA74-4618-9527-C8C5A4B15239}" name="Table1" displayName="Table1" ref="A1:G125" totalsRowShown="0">
+  <autoFilter ref="A1:G125" xr:uid="{20A5C34A-BA74-4618-9527-C8C5A4B15239}"/>
   <tableColumns count="7">
     <tableColumn id="2" xr3:uid="{8122BCC0-A9A0-4E8A-97F8-809454E87965}" name="Epic"/>
     <tableColumn id="3" xr3:uid="{62273C57-4035-404E-BD7F-DBE541848AF0}" name="Story"/>
-    <tableColumn id="4" xr3:uid="{F83CC626-5103-462B-9E71-70FF58ECD672}" name="Points" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{32A1D275-1575-4B11-A22D-5A36CD923379}" name="Estimated Hours" dataDxfId="4">
+    <tableColumn id="4" xr3:uid="{F83CC626-5103-462B-9E71-70FF58ECD672}" name="Points" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{32A1D275-1575-4B11-A22D-5A36CD923379}" name="Estimated Hours" dataDxfId="2">
       <calculatedColumnFormula>VLOOKUP(C2,Points!$A$1:$C$6,3,FALSE)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{E075E6CD-1DFD-47F5-B7CE-6A6F43BA85B6}" name="Completed"/>
-    <tableColumn id="8" xr3:uid="{775079EE-6981-4E34-B3C6-3629C5635AE6}" name="Completed Points" dataDxfId="3">
+    <tableColumn id="8" xr3:uid="{775079EE-6981-4E34-B3C6-3629C5635AE6}" name="Completed Points" dataDxfId="1">
       <calculatedColumnFormula>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{B8125C06-D59F-4CA7-817D-1DFF5C288455}" name="Completed Hours" dataDxfId="2">
+    <tableColumn id="7" xr3:uid="{B8125C06-D59F-4CA7-817D-1DFF5C288455}" name="Completed Hours" dataDxfId="0">
       <calculatedColumnFormula>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -623,8 +742,8 @@
   <tableColumns count="7">
     <tableColumn id="2" xr3:uid="{31CB5B43-DDC0-45F7-94FE-8435C1D008DA}" name="Epic"/>
     <tableColumn id="3" xr3:uid="{E8134CEE-EEF4-4605-A21F-CFF015B23BA2}" name="Story"/>
-    <tableColumn id="4" xr3:uid="{A8E050D4-AAEC-4516-ABB3-A0C110009E2F}" name="Points" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{AD6AC57F-E07B-42DB-850E-DEA524AE6E46}" name="Estimated Hours" dataDxfId="0">
+    <tableColumn id="4" xr3:uid="{A8E050D4-AAEC-4516-ABB3-A0C110009E2F}" name="Points" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{AD6AC57F-E07B-42DB-850E-DEA524AE6E46}" name="Estimated Hours" dataDxfId="4">
       <calculatedColumnFormula>VLOOKUP(C2,Points!$A$1:$C$6,3,FALSE)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{86F5B27A-D198-4848-ADB6-A7BEFFDB816F}" name="Completed"/>
@@ -640,9 +759,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -680,7 +799,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -786,7 +905,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -928,7 +1047,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -936,25 +1055,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F9D3302-E5F0-4E5C-9EB3-B74DDF37DF9D}">
-  <dimension ref="A1:G100"/>
+  <dimension ref="A1:G137"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B101" sqref="B101"/>
+      <pane ySplit="1" topLeftCell="A108" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B128" sqref="B128"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="34.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.46484375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.73046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.1328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.1328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -968,16 +1087,16 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F1" t="s">
+        <v>128</v>
+      </c>
+      <c r="G1" t="s">
         <v>119</v>
       </c>
-      <c r="F1" t="s">
-        <v>130</v>
-      </c>
-      <c r="G1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1003,7 +1122,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1029,7 +1148,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1055,7 +1174,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1081,7 +1200,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1107,7 +1226,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1133,7 +1252,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -1159,7 +1278,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -1185,7 +1304,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -1211,7 +1330,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -1237,7 +1356,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -1263,7 +1382,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -1289,7 +1408,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -1315,12 +1434,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>4</v>
       </c>
       <c r="B15" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C15" s="3">
         <v>1</v>
@@ -1341,7 +1460,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -1367,12 +1486,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>4</v>
       </c>
       <c r="B17" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C17" s="3">
         <v>2</v>
@@ -1393,12 +1512,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>4</v>
       </c>
       <c r="B18" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C18" s="3">
         <v>1</v>
@@ -1419,12 +1538,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>4</v>
       </c>
       <c r="B19" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C19" s="3">
         <v>1</v>
@@ -1445,7 +1564,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>4</v>
       </c>
@@ -1471,7 +1590,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>27</v>
       </c>
@@ -1497,7 +1616,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -1523,7 +1642,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -1549,7 +1668,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>27</v>
       </c>
@@ -1575,7 +1694,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>32</v>
       </c>
@@ -1601,7 +1720,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>32</v>
       </c>
@@ -1627,7 +1746,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>32</v>
       </c>
@@ -1653,7 +1772,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>32</v>
       </c>
@@ -1679,7 +1798,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>32</v>
       </c>
@@ -1705,7 +1824,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>32</v>
       </c>
@@ -1731,7 +1850,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>32</v>
       </c>
@@ -1757,7 +1876,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>40</v>
       </c>
@@ -1783,7 +1902,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>40</v>
       </c>
@@ -1809,7 +1928,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>40</v>
       </c>
@@ -1835,7 +1954,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>40</v>
       </c>
@@ -1861,7 +1980,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>40</v>
       </c>
@@ -1887,7 +2006,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>40</v>
       </c>
@@ -1913,7 +2032,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>47</v>
       </c>
@@ -1939,7 +2058,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>47</v>
       </c>
@@ -1965,7 +2084,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>47</v>
       </c>
@@ -1991,7 +2110,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>47</v>
       </c>
@@ -2017,7 +2136,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>47</v>
       </c>
@@ -2043,97 +2162,88 @@
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>53</v>
       </c>
       <c r="B43" t="s">
-        <v>54</v>
+        <v>146</v>
       </c>
       <c r="C43" s="3">
-        <v>2</v>
-      </c>
-      <c r="D43" s="3">
+        <v>5</v>
+      </c>
+      <c r="D43" s="13">
         <f>VLOOKUP(C43,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>8</v>
-      </c>
-      <c r="E43" t="b">
-        <v>1</v>
-      </c>
-      <c r="F43">
-        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>2</v>
-      </c>
-      <c r="G43">
-        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="F43" s="14">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="G43" s="14">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>53</v>
       </c>
       <c r="B44" t="s">
-        <v>55</v>
+        <v>147</v>
       </c>
       <c r="C44" s="3">
-        <v>2</v>
-      </c>
-      <c r="D44" s="3">
+        <v>5</v>
+      </c>
+      <c r="D44" s="13">
         <f>VLOOKUP(C44,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>8</v>
-      </c>
-      <c r="E44" t="b">
-        <v>1</v>
-      </c>
-      <c r="F44">
-        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>2</v>
-      </c>
-      <c r="G44">
-        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="F44" s="14">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="G44" s="14">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B45" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C45" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D45" s="3">
         <f>VLOOKUP(C45,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>16</v>
-      </c>
-      <c r="E45" t="b">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F45">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G45">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B46" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C46" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D46" s="3">
         <f>VLOOKUP(C46,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="F46">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
@@ -2144,12 +2254,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>56</v>
       </c>
       <c r="B47" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C47" s="3">
         <v>3</v>
@@ -2158,16 +2268,19 @@
         <f>VLOOKUP(C47,Points!$A$1:$C$6,3,FALSE)</f>
         <v>16</v>
       </c>
+      <c r="E47" t="b">
+        <v>1</v>
+      </c>
       <c r="F47">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G47">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>56</v>
       </c>
@@ -2193,133 +2306,142 @@
         <v>32</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>56</v>
       </c>
       <c r="B49" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C49" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D49" s="3">
         <f>VLOOKUP(C49,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>8</v>
+        <v>16</v>
+      </c>
+      <c r="E49" t="b">
+        <v>1</v>
       </c>
       <c r="F49">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G49">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
         <v>56</v>
       </c>
       <c r="B50" t="s">
-        <v>62</v>
+        <v>148</v>
       </c>
       <c r="C50" s="3">
         <v>2</v>
       </c>
-      <c r="D50" s="3">
+      <c r="D50" s="13">
         <f>VLOOKUP(C50,Points!$A$1:$C$6,3,FALSE)</f>
         <v>8</v>
       </c>
-      <c r="F50">
-        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
-      </c>
-      <c r="G50">
-        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E50" t="b">
+        <v>1</v>
+      </c>
+      <c r="F50" s="14">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>2</v>
+      </c>
+      <c r="G50" s="14">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>56</v>
       </c>
       <c r="B51" t="s">
+        <v>149</v>
+      </c>
+      <c r="C51" s="3">
+        <v>2</v>
+      </c>
+      <c r="D51" s="13">
+        <f>VLOOKUP(C51,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>8</v>
+      </c>
+      <c r="E51" t="b">
+        <v>1</v>
+      </c>
+      <c r="F51" s="14">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>2</v>
+      </c>
+      <c r="G51" s="14">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A52" t="s">
+        <v>56</v>
+      </c>
+      <c r="B52" t="s">
         <v>63</v>
       </c>
-      <c r="C51" s="3">
-        <v>2</v>
-      </c>
-      <c r="D51" s="3">
-        <f>VLOOKUP(C51,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>8</v>
-      </c>
-      <c r="F51">
-        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
-      </c>
-      <c r="G51">
-        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>64</v>
-      </c>
-      <c r="B52" t="s">
-        <v>65</v>
-      </c>
       <c r="C52" s="3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D52" s="3">
         <f>VLOOKUP(C52,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="E52" t="b">
         <v>1</v>
       </c>
       <c r="F52">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G52">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>32</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="B53" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C53" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D53" s="3">
         <f>VLOOKUP(C53,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E53" t="b">
         <v>1</v>
       </c>
       <c r="F53">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G53">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="B54" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C54" s="3">
         <v>5</v>
@@ -2328,73 +2450,67 @@
         <f>VLOOKUP(C54,Points!$A$1:$C$6,3,FALSE)</f>
         <v>32</v>
       </c>
-      <c r="E54" t="b">
-        <v>1</v>
-      </c>
       <c r="F54">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G54">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>32</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="B55" t="s">
-        <v>68</v>
+        <v>150</v>
       </c>
       <c r="C55" s="3">
         <v>2</v>
       </c>
-      <c r="D55" s="3">
+      <c r="D55" s="13">
         <f>VLOOKUP(C55,Points!$A$1:$C$6,3,FALSE)</f>
         <v>8</v>
       </c>
-      <c r="F55">
-        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
-      </c>
-      <c r="G55">
-        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F55" s="14">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="G55" s="14">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="B56" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="C56" s="3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D56" s="3">
         <f>VLOOKUP(C56,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>32</v>
-      </c>
-      <c r="E56" t="b">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F56">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G56">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>32</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B57" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C57" s="3">
         <v>5</v>
@@ -2415,58 +2531,64 @@
         <v>32</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B58" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C58" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D58" s="3">
         <f>VLOOKUP(C58,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>32</v>
+        <v>16</v>
+      </c>
+      <c r="E58" t="b">
+        <v>1</v>
       </c>
       <c r="F58">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G58">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B59" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C59" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D59" s="3">
         <f>VLOOKUP(C59,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>16</v>
+        <v>32</v>
+      </c>
+      <c r="E59" t="b">
+        <v>1</v>
       </c>
       <c r="F59">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G59">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B60" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C60" s="3">
         <v>5</v>
@@ -2484,12 +2606,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B61" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C61" s="3">
         <v>5</v>
@@ -2510,12 +2632,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B62" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C62" s="3">
         <v>5</v>
@@ -2536,19 +2658,19 @@
         <v>32</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B63" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C63" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D63" s="3">
         <f>VLOOKUP(C63,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="F63">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
@@ -2559,12 +2681,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B64" t="s">
-        <v>140</v>
+        <v>151</v>
       </c>
       <c r="C64" s="3">
         <v>5</v>
@@ -2573,76 +2695,67 @@
         <f>VLOOKUP(C64,Points!$A$1:$C$6,3,FALSE)</f>
         <v>32</v>
       </c>
-      <c r="E64" t="b">
-        <v>1</v>
-      </c>
       <c r="F64">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G64">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>32</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="B65" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="C65" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D65" s="3">
         <f>VLOOKUP(C65,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>16</v>
-      </c>
-      <c r="E65" t="b">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="F65">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G65">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="B66" t="s">
-        <v>81</v>
+        <v>152</v>
       </c>
       <c r="C66" s="3">
         <v>5</v>
       </c>
-      <c r="D66" s="3">
+      <c r="D66" s="13">
         <f>VLOOKUP(C66,Points!$A$1:$C$6,3,FALSE)</f>
         <v>32</v>
       </c>
-      <c r="E66" t="b">
-        <v>1</v>
-      </c>
-      <c r="F66">
-        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>5</v>
-      </c>
-      <c r="G66">
-        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>32</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F66" s="14">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="G66" s="14">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="B67" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="C67" s="3">
         <v>5</v>
@@ -2651,44 +2764,50 @@
         <f>VLOOKUP(C67,Points!$A$1:$C$6,3,FALSE)</f>
         <v>32</v>
       </c>
+      <c r="E67" t="b">
+        <v>1</v>
+      </c>
       <c r="F67">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G67">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="B68" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="C68" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D68" s="3">
         <f>VLOOKUP(C68,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>16</v>
+        <v>32</v>
+      </c>
+      <c r="E68" t="b">
+        <v>1</v>
       </c>
       <c r="F68">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G68">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="B69" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="C69" s="3">
         <v>3</v>
@@ -2697,21 +2816,24 @@
         <f>VLOOKUP(C69,Points!$A$1:$C$6,3,FALSE)</f>
         <v>16</v>
       </c>
+      <c r="E69" t="b">
+        <v>1</v>
+      </c>
       <c r="F69">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G69">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="B70" t="s">
-        <v>86</v>
+        <v>138</v>
       </c>
       <c r="C70" s="3">
         <v>5</v>
@@ -2720,96 +2842,99 @@
         <f>VLOOKUP(C70,Points!$A$1:$C$6,3,FALSE)</f>
         <v>32</v>
       </c>
+      <c r="E70" t="b">
+        <v>1</v>
+      </c>
       <c r="F70">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G70">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B71" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="C71" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D71" s="3">
         <f>VLOOKUP(C71,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>32</v>
+        <v>16</v>
+      </c>
+      <c r="E71" t="b">
+        <v>1</v>
       </c>
       <c r="F71">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G71">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="B72" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="C72" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D72" s="3">
         <f>VLOOKUP(C72,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="E72" t="b">
         <v>1</v>
       </c>
       <c r="F72">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G72">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="B73" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="C73" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D73" s="3">
         <f>VLOOKUP(C73,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>16</v>
-      </c>
-      <c r="E73" t="b">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="F73">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G73">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="B74" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="C74" s="3">
         <v>3</v>
@@ -2818,24 +2943,21 @@
         <f>VLOOKUP(C74,Points!$A$1:$C$6,3,FALSE)</f>
         <v>16</v>
       </c>
-      <c r="E74" t="b">
-        <v>1</v>
-      </c>
       <c r="F74">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G74">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="B75" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="C75" s="3">
         <v>3</v>
@@ -2844,54 +2966,54 @@
         <f>VLOOKUP(C75,Points!$A$1:$C$6,3,FALSE)</f>
         <v>16</v>
       </c>
-      <c r="E75" t="b">
-        <v>1</v>
-      </c>
       <c r="F75">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G75">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
-        <v>141</v>
+        <v>81</v>
       </c>
       <c r="B76" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="C76" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D76" s="3">
         <f>VLOOKUP(C76,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>16</v>
+        <v>32</v>
+      </c>
+      <c r="E76" t="b">
+        <v>1</v>
       </c>
       <c r="F76">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G76">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
-        <v>141</v>
+        <v>81</v>
       </c>
       <c r="B77" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="C77" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D77" s="3">
         <f>VLOOKUP(C77,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="F77">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
@@ -2902,12 +3024,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
-        <v>141</v>
+        <v>87</v>
       </c>
       <c r="B78" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="C78" s="3">
         <v>3</v>
@@ -2916,21 +3038,24 @@
         <f>VLOOKUP(C78,Points!$A$1:$C$6,3,FALSE)</f>
         <v>16</v>
       </c>
+      <c r="E78" t="b">
+        <v>1</v>
+      </c>
       <c r="F78">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G78">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
-        <v>141</v>
+        <v>87</v>
       </c>
       <c r="B79" t="s">
-        <v>142</v>
+        <v>89</v>
       </c>
       <c r="C79" s="3">
         <v>3</v>
@@ -2939,21 +3064,24 @@
         <f>VLOOKUP(C79,Points!$A$1:$C$6,3,FALSE)</f>
         <v>16</v>
       </c>
+      <c r="E79" t="b">
+        <v>1</v>
+      </c>
       <c r="F79">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G79">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
-        <v>141</v>
+        <v>87</v>
       </c>
       <c r="B80" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C80" s="3">
         <v>3</v>
@@ -2962,21 +3090,24 @@
         <f>VLOOKUP(C80,Points!$A$1:$C$6,3,FALSE)</f>
         <v>16</v>
       </c>
+      <c r="E80" t="b">
+        <v>1</v>
+      </c>
       <c r="F80">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G80">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
-        <v>141</v>
+        <v>87</v>
       </c>
       <c r="B81" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C81" s="3">
         <v>3</v>
@@ -2985,16 +3116,19 @@
         <f>VLOOKUP(C81,Points!$A$1:$C$6,3,FALSE)</f>
         <v>16</v>
       </c>
+      <c r="E81" t="b">
+        <v>1</v>
+      </c>
       <c r="F81">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G81">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
         <v>141</v>
       </c>
@@ -3017,9 +3151,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B83" t="s">
         <v>99</v>
@@ -3040,19 +3174,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B84" t="s">
         <v>100</v>
       </c>
       <c r="C84" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D84" s="3">
         <f>VLOOKUP(C84,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="F84">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
@@ -3063,19 +3197,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B85" t="s">
         <v>101</v>
       </c>
       <c r="C85" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D85" s="3">
         <f>VLOOKUP(C85,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="F85">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
@@ -3086,19 +3220,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B86" t="s">
-        <v>102</v>
+        <v>142</v>
       </c>
       <c r="C86" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D86" s="3">
         <f>VLOOKUP(C86,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="F86">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
@@ -3109,19 +3243,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B87" t="s">
-        <v>144</v>
+        <v>102</v>
       </c>
       <c r="C87" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D87" s="3">
         <f>VLOOKUP(C87,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="F87">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
@@ -3132,19 +3266,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B88" t="s">
         <v>103</v>
       </c>
       <c r="C88" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D88" s="3">
         <f>VLOOKUP(C88,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F88">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
@@ -3155,19 +3289,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B89" t="s">
         <v>104</v>
       </c>
       <c r="C89" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D89" s="3">
         <f>VLOOKUP(C89,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F89">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
@@ -3178,19 +3312,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B90" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="C90" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D90" s="3">
         <f>VLOOKUP(C90,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="F90">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
@@ -3201,102 +3335,959 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A92" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="B92" s="4"/>
-      <c r="C92" s="5">
-        <f>SUM(C2:C91)</f>
-        <v>250</v>
-      </c>
-      <c r="D92" s="5">
-        <f>SUM(D2:D91)</f>
-        <v>1340</v>
-      </c>
-      <c r="F92" s="4">
-        <f>SUM(F2:F91)</f>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A91" t="s">
+        <v>139</v>
+      </c>
+      <c r="B91" t="s">
+        <v>93</v>
+      </c>
+      <c r="C91" s="3">
+        <v>3</v>
+      </c>
+      <c r="D91" s="3">
+        <f>VLOOKUP(C91,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>16</v>
+      </c>
+      <c r="F91">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="G91">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A92" t="s">
+        <v>139</v>
+      </c>
+      <c r="B92" t="s">
+        <v>94</v>
+      </c>
+      <c r="C92" s="3">
+        <v>3</v>
+      </c>
+      <c r="D92" s="3">
+        <f>VLOOKUP(C92,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>16</v>
+      </c>
+      <c r="F92">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="G92">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A93" t="s">
+        <v>139</v>
+      </c>
+      <c r="B93" t="s">
+        <v>140</v>
+      </c>
+      <c r="C93" s="3">
+        <v>3</v>
+      </c>
+      <c r="D93" s="3">
+        <f>VLOOKUP(C93,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>16</v>
+      </c>
+      <c r="F93">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="G93">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A94" t="s">
+        <v>139</v>
+      </c>
+      <c r="B94" t="s">
+        <v>95</v>
+      </c>
+      <c r="C94" s="3">
+        <v>3</v>
+      </c>
+      <c r="D94" s="3">
+        <f>VLOOKUP(C94,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>16</v>
+      </c>
+      <c r="F94">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="G94">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A95" t="s">
+        <v>139</v>
+      </c>
+      <c r="B95" t="s">
+        <v>96</v>
+      </c>
+      <c r="C95" s="3">
+        <v>1</v>
+      </c>
+      <c r="D95" s="3">
+        <f>VLOOKUP(C95,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="F95">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="G95">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A96" t="s">
+        <v>139</v>
+      </c>
+      <c r="B96" t="s">
+        <v>97</v>
+      </c>
+      <c r="C96" s="3">
+        <v>1</v>
+      </c>
+      <c r="D96" s="3">
+        <f>VLOOKUP(C96,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="F96">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="G96">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A97" t="s">
+        <v>153</v>
+      </c>
+      <c r="B97" t="s">
+        <v>154</v>
+      </c>
+      <c r="C97" s="3">
+        <v>5</v>
+      </c>
+      <c r="D97" s="13">
+        <f>VLOOKUP(C97,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>32</v>
+      </c>
+      <c r="E97" t="b">
+        <v>1</v>
+      </c>
+      <c r="F97" s="14">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>5</v>
+      </c>
+      <c r="G97" s="14">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A98" t="s">
+        <v>153</v>
+      </c>
+      <c r="B98" t="s">
+        <v>155</v>
+      </c>
+      <c r="C98" s="3">
+        <v>1</v>
+      </c>
+      <c r="D98" s="13">
+        <f>VLOOKUP(C98,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="E98" t="b">
+        <v>1</v>
+      </c>
+      <c r="F98" s="14">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>1</v>
+      </c>
+      <c r="G98" s="14">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A99" t="s">
+        <v>153</v>
+      </c>
+      <c r="B99" t="s">
+        <v>156</v>
+      </c>
+      <c r="C99" s="3">
+        <v>1</v>
+      </c>
+      <c r="D99" s="13">
+        <f>VLOOKUP(C99,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="E99" t="b">
+        <v>1</v>
+      </c>
+      <c r="F99" s="14">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>1</v>
+      </c>
+      <c r="G99" s="14">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A100" t="s">
+        <v>153</v>
+      </c>
+      <c r="B100" t="s">
+        <v>157</v>
+      </c>
+      <c r="C100" s="3">
+        <v>1</v>
+      </c>
+      <c r="D100" s="13">
+        <f>VLOOKUP(C100,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="E100" t="b">
+        <v>1</v>
+      </c>
+      <c r="F100" s="14">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>1</v>
+      </c>
+      <c r="G100" s="14">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A101" t="s">
+        <v>153</v>
+      </c>
+      <c r="B101" t="s">
+        <v>158</v>
+      </c>
+      <c r="C101" s="3">
+        <v>1</v>
+      </c>
+      <c r="D101" s="13">
+        <f>VLOOKUP(C101,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="E101" t="b">
+        <v>1</v>
+      </c>
+      <c r="F101" s="14">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>1</v>
+      </c>
+      <c r="G101" s="14">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A102" t="s">
+        <v>153</v>
+      </c>
+      <c r="B102" t="s">
+        <v>159</v>
+      </c>
+      <c r="C102" s="3">
+        <v>3</v>
+      </c>
+      <c r="D102" s="13">
+        <f>VLOOKUP(C102,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>16</v>
+      </c>
+      <c r="E102" t="b">
+        <v>1</v>
+      </c>
+      <c r="F102" s="14">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>3</v>
+      </c>
+      <c r="G102" s="14">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A103" t="s">
+        <v>153</v>
+      </c>
+      <c r="B103" t="s">
+        <v>160</v>
+      </c>
+      <c r="C103" s="3">
+        <v>1</v>
+      </c>
+      <c r="D103" s="13">
+        <f>VLOOKUP(C103,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="E103" t="b">
+        <v>1</v>
+      </c>
+      <c r="F103" s="14">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>1</v>
+      </c>
+      <c r="G103" s="14">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A104" t="s">
+        <v>153</v>
+      </c>
+      <c r="B104" t="s">
+        <v>161</v>
+      </c>
+      <c r="C104" s="3">
+        <v>1</v>
+      </c>
+      <c r="D104" s="13">
+        <f>VLOOKUP(C104,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="E104" t="b">
+        <v>1</v>
+      </c>
+      <c r="F104" s="14">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>1</v>
+      </c>
+      <c r="G104" s="14">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A105" t="s">
+        <v>153</v>
+      </c>
+      <c r="B105" t="s">
+        <v>162</v>
+      </c>
+      <c r="C105" s="3">
+        <v>1</v>
+      </c>
+      <c r="D105" s="13">
+        <f>VLOOKUP(C105,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="E105" t="b">
+        <v>1</v>
+      </c>
+      <c r="F105" s="14">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>1</v>
+      </c>
+      <c r="G105" s="14">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A106" t="s">
+        <v>153</v>
+      </c>
+      <c r="B106" t="s">
         <v>163</v>
       </c>
-      <c r="G92">
-        <f>SUM(G2:G91)</f>
-        <v>884</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A93" s="6"/>
-      <c r="B93" s="4"/>
-      <c r="C93" s="5"/>
-      <c r="D93" s="5"/>
-      <c r="G93" s="4"/>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A94" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="B94" s="11">
-        <f ca="1">B96+B95</f>
-        <v>63.665158371040725</v>
-      </c>
-      <c r="D94" s="7"/>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A95" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="B95" s="11">
-        <f ca="1">(D92-G92)/B100</f>
-        <v>21.665158371040725</v>
-      </c>
-      <c r="D95" s="7"/>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A96" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="B96" s="4">
+      <c r="C106" s="3">
+        <v>1</v>
+      </c>
+      <c r="D106" s="13">
+        <f>VLOOKUP(C106,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="E106" t="b">
+        <v>1</v>
+      </c>
+      <c r="F106" s="14">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>1</v>
+      </c>
+      <c r="G106" s="14">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A107" t="s">
+        <v>153</v>
+      </c>
+      <c r="B107" t="s">
+        <v>164</v>
+      </c>
+      <c r="C107" s="3">
+        <v>1</v>
+      </c>
+      <c r="D107" s="13">
+        <f>VLOOKUP(C107,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="E107" t="b">
+        <v>1</v>
+      </c>
+      <c r="F107" s="14">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>1</v>
+      </c>
+      <c r="G107" s="14">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A108" t="s">
+        <v>153</v>
+      </c>
+      <c r="B108" t="s">
+        <v>165</v>
+      </c>
+      <c r="C108" s="3">
+        <v>1</v>
+      </c>
+      <c r="D108" s="13">
+        <f>VLOOKUP(C108,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="F108" s="14">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="G108" s="14">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A109" t="s">
+        <v>153</v>
+      </c>
+      <c r="B109" t="s">
+        <v>166</v>
+      </c>
+      <c r="C109" s="3">
+        <v>1</v>
+      </c>
+      <c r="D109" s="13">
+        <f>VLOOKUP(C109,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="F109" s="14">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="G109" s="14">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A110" t="s">
+        <v>153</v>
+      </c>
+      <c r="B110" t="s">
+        <v>167</v>
+      </c>
+      <c r="C110" s="3">
+        <v>1</v>
+      </c>
+      <c r="D110" s="13">
+        <f>VLOOKUP(C110,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="F110" s="14">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="G110" s="14">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A111" t="s">
+        <v>153</v>
+      </c>
+      <c r="B111" t="s">
+        <v>168</v>
+      </c>
+      <c r="C111" s="3">
+        <v>1</v>
+      </c>
+      <c r="D111" s="13">
+        <f>VLOOKUP(C111,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="F111" s="14">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="G111" s="14">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A112" t="s">
+        <v>153</v>
+      </c>
+      <c r="B112" t="s">
+        <v>169</v>
+      </c>
+      <c r="C112" s="3">
+        <v>1</v>
+      </c>
+      <c r="D112" s="13">
+        <f>VLOOKUP(C112,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="F112" s="14">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="G112" s="14">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A113" t="s">
+        <v>153</v>
+      </c>
+      <c r="B113" t="s">
+        <v>170</v>
+      </c>
+      <c r="C113" s="3">
+        <v>2</v>
+      </c>
+      <c r="D113" s="13">
+        <f>VLOOKUP(C113,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>8</v>
+      </c>
+      <c r="F113" s="14">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="G113" s="14">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A114" t="s">
+        <v>153</v>
+      </c>
+      <c r="B114" t="s">
+        <v>171</v>
+      </c>
+      <c r="C114" s="3">
+        <v>1</v>
+      </c>
+      <c r="D114" s="13">
+        <f>VLOOKUP(C114,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="F114" s="14">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="G114" s="14">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A115" t="s">
+        <v>153</v>
+      </c>
+      <c r="B115" t="s">
+        <v>172</v>
+      </c>
+      <c r="C115" s="3">
+        <v>1</v>
+      </c>
+      <c r="D115" s="13">
+        <f>VLOOKUP(C115,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="F115" s="14">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="G115" s="14">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A116" t="s">
+        <v>153</v>
+      </c>
+      <c r="B116" t="s">
+        <v>173</v>
+      </c>
+      <c r="C116" s="3">
+        <v>1</v>
+      </c>
+      <c r="D116" s="13">
+        <f>VLOOKUP(C116,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="F116" s="14">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="G116" s="14">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A117" t="s">
+        <v>153</v>
+      </c>
+      <c r="B117" t="s">
+        <v>174</v>
+      </c>
+      <c r="C117" s="3">
+        <v>1</v>
+      </c>
+      <c r="D117" s="13">
+        <f>VLOOKUP(C117,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="F117" s="14">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="G117" s="14">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A118" t="s">
+        <v>153</v>
+      </c>
+      <c r="B118" t="s">
+        <v>175</v>
+      </c>
+      <c r="C118" s="3">
+        <v>5</v>
+      </c>
+      <c r="D118" s="13">
+        <f>VLOOKUP(C118,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>32</v>
+      </c>
+      <c r="F118" s="14">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="G118" s="14">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A119" t="s">
+        <v>153</v>
+      </c>
+      <c r="B119" t="s">
+        <v>176</v>
+      </c>
+      <c r="C119" s="3">
+        <v>3</v>
+      </c>
+      <c r="D119" s="13">
+        <f>VLOOKUP(C119,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>16</v>
+      </c>
+      <c r="F119" s="14">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="G119" s="14">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A120" t="s">
+        <v>153</v>
+      </c>
+      <c r="B120" t="s">
+        <v>177</v>
+      </c>
+      <c r="C120" s="3">
+        <v>3</v>
+      </c>
+      <c r="D120" s="13">
+        <f>VLOOKUP(C120,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>16</v>
+      </c>
+      <c r="F120" s="14">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="G120" s="14">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A121" t="s">
+        <v>153</v>
+      </c>
+      <c r="B121" t="s">
+        <v>178</v>
+      </c>
+      <c r="C121" s="3">
+        <v>1</v>
+      </c>
+      <c r="D121" s="13">
+        <f>VLOOKUP(C121,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="F121" s="14">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="G121" s="14">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A122" t="s">
+        <v>153</v>
+      </c>
+      <c r="B122" t="s">
+        <v>179</v>
+      </c>
+      <c r="C122" s="3">
+        <v>2</v>
+      </c>
+      <c r="D122" s="13">
+        <f>VLOOKUP(C122,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>8</v>
+      </c>
+      <c r="F122" s="14">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="G122" s="14">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A123" t="s">
+        <v>153</v>
+      </c>
+      <c r="B123" t="s">
+        <v>180</v>
+      </c>
+      <c r="C123" s="3">
+        <v>1</v>
+      </c>
+      <c r="D123" s="13">
+        <f>VLOOKUP(C123,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="F123" s="14">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="G123" s="14">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A124" t="s">
+        <v>153</v>
+      </c>
+      <c r="B124" t="s">
+        <v>181</v>
+      </c>
+      <c r="C124" s="3">
+        <v>1</v>
+      </c>
+      <c r="D124" s="13">
+        <f>VLOOKUP(C124,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="F124" s="14">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="G124" s="14">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A125" t="s">
+        <v>153</v>
+      </c>
+      <c r="B125" t="s">
+        <v>182</v>
+      </c>
+      <c r="C125" s="3">
+        <v>3</v>
+      </c>
+      <c r="D125" s="13">
+        <f>VLOOKUP(C125,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>16</v>
+      </c>
+      <c r="F125" s="14">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="G125" s="14">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A127" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B127" s="4"/>
+      <c r="C127" s="5">
+        <f>SUM(C2:C126)</f>
+        <v>324</v>
+      </c>
+      <c r="D127" s="5">
+        <f>SUM(D2:D126)</f>
+        <v>1752</v>
+      </c>
+      <c r="F127" s="4">
+        <f>SUM(F2:F126)</f>
+        <v>195</v>
+      </c>
+      <c r="G127" s="4">
+        <f>SUM(G2:G126)</f>
+        <v>1048</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A128" s="6"/>
+      <c r="B128" s="4"/>
+      <c r="C128" s="5"/>
+      <c r="D128" s="5"/>
+      <c r="G128" s="4"/>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A129" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="B129" s="11">
+        <f ca="1">B131+B130</f>
+        <v>128.29007633587787</v>
+      </c>
+      <c r="D129" s="7"/>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A130" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="B130" s="11">
+        <f ca="1">(D127-G127)/B137</f>
+        <v>38.290076335877863</v>
+      </c>
+      <c r="D130" s="7"/>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A131" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="B131" s="4">
         <f ca="1">FLOOR(((TODAY()-Variables!B2)/7),1)</f>
-        <v>42</v>
-      </c>
-      <c r="D96" s="7"/>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A97" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="B97" s="12">
+        <v>90</v>
+      </c>
+      <c r="D131" s="7"/>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A132" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="B132" s="4">
+        <v>33</v>
+      </c>
+      <c r="D132" s="7"/>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A133" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="B133" s="4">
+        <f ca="1">B131-B132</f>
+        <v>57</v>
+      </c>
+      <c r="D133" s="7"/>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A134" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B134" s="12">
         <f>Variables!B2</f>
         <v>44892</v>
       </c>
-      <c r="D97" s="7"/>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A98" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="B98" s="12">
-        <f ca="1">TODAY()+ (B95*7)</f>
-        <v>45338.656108597286</v>
-      </c>
-      <c r="D98" s="9"/>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A99" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="B99" s="11">
-        <f ca="1">F92/B96</f>
-        <v>3.8809523809523809</v>
-      </c>
-      <c r="F99" s="10"/>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A100" s="6" t="s">
+      <c r="D134" s="7"/>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A135" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="B135" s="12">
+        <f ca="1">TODAY()+ (B130*7)</f>
+        <v>45793.030534351143</v>
+      </c>
+      <c r="D135" s="9"/>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A136" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="B100" s="4">
-        <f ca="1">G92/B96</f>
-        <v>21.047619047619047</v>
+      <c r="B136" s="11">
+        <f ca="1">F127/B133</f>
+        <v>3.4210526315789473</v>
+      </c>
+      <c r="F136" s="10"/>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A137" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="B137" s="15">
+        <f ca="1">G127/B133</f>
+        <v>18.385964912280702</v>
       </c>
     </row>
   </sheetData>
@@ -3316,18 +4307,18 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.1328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.1328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3341,21 +4332,21 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F1" t="s">
+        <v>128</v>
+      </c>
+      <c r="G1" t="s">
         <v>119</v>
       </c>
-      <c r="F1" t="s">
-        <v>130</v>
-      </c>
-      <c r="G1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C2" s="3">
         <v>5</v>
@@ -3373,12 +4364,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B3" t="s">
         <v>107</v>
-      </c>
-      <c r="B3" t="s">
-        <v>108</v>
       </c>
       <c r="C3" s="3">
         <v>3</v>
@@ -3396,12 +4387,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C4" s="3">
         <v>5</v>
@@ -3419,12 +4410,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B5" t="s">
         <v>110</v>
-      </c>
-      <c r="B5" t="s">
-        <v>111</v>
       </c>
       <c r="C5" s="3">
         <v>2</v>
@@ -3442,12 +4433,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C6" s="3">
         <v>2</v>
@@ -3465,12 +4456,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C7" s="3">
         <v>5</v>
@@ -3488,12 +4479,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C8" s="3">
         <v>5</v>
@@ -3511,12 +4502,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C9" s="3">
         <v>5</v>
@@ -3534,9 +4525,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C11">
         <f>SUM(C2:C10)</f>
@@ -3560,17 +4551,17 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="3"/>
+    <col min="1" max="1" width="6.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.1328125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3581,7 +4572,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3592,7 +4583,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3603,7 +4594,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3614,7 +4605,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>5</v>
       </c>
@@ -3625,7 +4616,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>8</v>
       </c>
@@ -3649,47 +4640,47 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
         <v>137</v>
-      </c>
-      <c r="B2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>138</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>139</v>
       </c>
       <c r="B4">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B6" s="4">
         <f>SUM(B2:B4)</f>
@@ -3709,22 +4700,22 @@
       <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
         <v>122</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>123</v>
       </c>
       <c r="B2" s="8">
         <v>44892</v>

</xml_diff>

<commit_message>
Update NuGet Package Versions and Tests
</commit_message>
<xml_diff>
--- a/Documentation/Design/Estimates.xlsx
+++ b/Documentation/Design/Estimates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_git\BedBrigadeNationalV8\Documentation\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA0DFCF1-55C8-438A-8175-C8459DF203C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B779A938-9CB7-4C37-9BA0-34CFE43F3B29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="30" windowWidth="28770" windowHeight="15450" xr2:uid="{D27F5AFA-C88C-4A2F-A896-BFED2572A1C7}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D27F5AFA-C88C-4A2F-A896-BFED2572A1C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Estimates" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="190">
   <si>
     <t>Epic</t>
   </si>
@@ -604,13 +604,19 @@
   </si>
   <si>
     <t>Blazor 9 Change Render Mode</t>
+  </si>
+  <si>
+    <t>Project Percent Complete</t>
+  </si>
+  <si>
+    <t>Remaining Hours</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -629,6 +635,13 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -657,10 +670,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -687,13 +701,11 @@
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="6">
     <dxf>
@@ -1070,16 +1082,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F9D3302-E5F0-4E5C-9EB3-B74DDF37DF9D}">
-  <dimension ref="A1:G142"/>
+  <dimension ref="A1:G144"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A100" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B121" sqref="B121"/>
+      <pane ySplit="1" topLeftCell="A118" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B150" sqref="B150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="51.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.140625" style="3" bestFit="1" customWidth="1"/>
@@ -4158,15 +4170,15 @@
       <c r="C124" s="3">
         <v>2</v>
       </c>
-      <c r="D124" s="14">
+      <c r="D124" s="3">
         <f>VLOOKUP(C124,Points!$A$1:$C$6,3,FALSE)</f>
         <v>8</v>
       </c>
-      <c r="F124" s="15">
-        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
-      </c>
-      <c r="G124" s="15">
+      <c r="F124">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="G124">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
         <v>0</v>
       </c>
@@ -4181,15 +4193,15 @@
       <c r="C125" s="3">
         <v>2</v>
       </c>
-      <c r="D125" s="14">
+      <c r="D125" s="3">
         <f>VLOOKUP(C125,Points!$A$1:$C$6,3,FALSE)</f>
         <v>8</v>
       </c>
-      <c r="F125" s="15">
-        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
-      </c>
-      <c r="G125" s="15">
+      <c r="F125">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="G125">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
         <v>0</v>
       </c>
@@ -4204,15 +4216,15 @@
       <c r="C126" s="3">
         <v>1</v>
       </c>
-      <c r="D126" s="14">
+      <c r="D126" s="3">
         <f>VLOOKUP(C126,Points!$A$1:$C$6,3,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="F126" s="15">
-        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
-      </c>
-      <c r="G126" s="15">
+      <c r="F126">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="G126">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
         <v>0</v>
       </c>
@@ -4227,15 +4239,15 @@
       <c r="C127" s="3">
         <v>2</v>
       </c>
-      <c r="D127" s="14">
+      <c r="D127" s="3">
         <f>VLOOKUP(C127,Points!$A$1:$C$6,3,FALSE)</f>
         <v>8</v>
       </c>
-      <c r="F127" s="15">
-        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
-      </c>
-      <c r="G127" s="15">
+      <c r="F127">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="G127">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
         <v>0</v>
       </c>
@@ -4250,15 +4262,15 @@
       <c r="C128" s="3">
         <v>2</v>
       </c>
-      <c r="D128" s="14">
+      <c r="D128" s="3">
         <f>VLOOKUP(C128,Points!$A$1:$C$6,3,FALSE)</f>
         <v>8</v>
       </c>
-      <c r="F128" s="15">
-        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
-      </c>
-      <c r="G128" s="15">
+      <c r="F128">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="G128">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
         <v>0</v>
       </c>
@@ -4273,15 +4285,15 @@
       <c r="C129" s="3">
         <v>2</v>
       </c>
-      <c r="D129" s="14">
+      <c r="D129" s="3">
         <f>VLOOKUP(C129,Points!$A$1:$C$6,3,FALSE)</f>
         <v>8</v>
       </c>
-      <c r="F129" s="15">
-        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
-      </c>
-      <c r="G129" s="15">
+      <c r="F129">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="G129">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
         <v>0</v>
       </c>
@@ -4403,7 +4415,7 @@
       </c>
       <c r="B140" s="12">
         <f ca="1">TODAY()+ (B135*7)</f>
-        <v>45811.431818181816</v>
+        <v>45812.431818181816</v>
       </c>
       <c r="D140" s="9"/>
     </row>
@@ -4424,6 +4436,24 @@
       <c r="B142" s="13">
         <f ca="1">G132/B138</f>
         <v>18.206896551724139</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A143" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="B143" s="11">
+        <f>D132-G132</f>
+        <v>732</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A144" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="B144" s="14">
+        <f>G132/D132</f>
+        <v>0.59060402684563762</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Project Status and fix margins for mobile
</commit_message>
<xml_diff>
--- a/Documentation/Design/Estimates.xlsx
+++ b/Documentation/Design/Estimates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_git\BedBrigadeNationalV8\Documentation\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60B4C65F-7057-4816-B4AA-5DADA762BD43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{723037DE-83E5-4B56-B2EE-1D601E6CABB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D27F5AFA-C88C-4A2F-A896-BFED2572A1C7}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="208">
   <si>
     <t>Epic</t>
   </si>
@@ -285,9 +285,6 @@
     <t>Grove City Donate</t>
   </si>
   <si>
-    <t>Setup Paypal IPN</t>
-  </si>
-  <si>
     <t>Polaris Donate</t>
   </si>
   <si>
@@ -459,9 +456,6 @@
     <t>Manage Delivery Checklist</t>
   </si>
   <si>
-    <t>Scheduled Deliveries Email Checklist</t>
-  </si>
-  <si>
     <t>Tech Debt</t>
   </si>
   <si>
@@ -634,6 +628,42 @@
   </si>
   <si>
     <t>Date</t>
+  </si>
+  <si>
+    <t>Use Animate.css and Wow.js</t>
+  </si>
+  <si>
+    <t>Migration Deployment Setup Database and Preload</t>
+  </si>
+  <si>
+    <t>Improve Performance</t>
+  </si>
+  <si>
+    <t>Edit EmailTaxForm</t>
+  </si>
+  <si>
+    <t>Create Custom Authentication</t>
+  </si>
+  <si>
+    <t>Create Server Information Page</t>
+  </si>
+  <si>
+    <t>Mobile Bed Brigade Near Me</t>
+  </si>
+  <si>
+    <t>Mobile After Submit Bed Request</t>
+  </si>
+  <si>
+    <t>Mobile after Contact Us</t>
+  </si>
+  <si>
+    <t>Mobile after Submit Volunteer</t>
+  </si>
+  <si>
+    <t>Admin Mobile Margin and Padding</t>
+  </si>
+  <si>
+    <t>Manage Users Unusable in Mobile</t>
   </si>
 </sst>
 </file>
@@ -865,10 +895,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Burn Down'!$B$2:$B$6</c:f>
+              <c:f>'Burn Down'!$B$2:$B$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>56</c:v>
                 </c:pt>
@@ -884,15 +914,18 @@
                 <c:pt idx="4">
                   <c:v>60</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>62</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Burn Down'!$C$2:$C$6</c:f>
+              <c:f>'Burn Down'!$C$2:$C$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>568</c:v>
                 </c:pt>
@@ -907,6 +940,9 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>664</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>472</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1795,8 +1831,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{20A5C34A-BA74-4618-9527-C8C5A4B15239}" name="Table1" displayName="Table1" ref="A1:G147" totalsRowShown="0">
-  <autoFilter ref="A1:G147" xr:uid="{20A5C34A-BA74-4618-9527-C8C5A4B15239}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{20A5C34A-BA74-4618-9527-C8C5A4B15239}" name="Table1" displayName="Table1" ref="A1:G161" totalsRowShown="0">
+  <autoFilter ref="A1:G161" xr:uid="{20A5C34A-BA74-4618-9527-C8C5A4B15239}"/>
   <tableColumns count="7">
     <tableColumn id="2" xr3:uid="{8122BCC0-A9A0-4E8A-97F8-809454E87965}" name="Epic"/>
     <tableColumn id="3" xr3:uid="{62273C57-4035-404E-BD7F-DBE541848AF0}" name="Story"/>
@@ -2113,11 +2149,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F9D3302-E5F0-4E5C-9EB3-B74DDF37DF9D}">
-  <dimension ref="A1:G161"/>
+  <dimension ref="A1:G175"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B155" sqref="B155"/>
+      <pane ySplit="1" topLeftCell="A134" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B174" sqref="B174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2145,13 +2181,13 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F1" t="s">
+        <v>115</v>
+      </c>
+      <c r="G1" t="s">
         <v>106</v>
-      </c>
-      <c r="F1" t="s">
-        <v>116</v>
-      </c>
-      <c r="G1" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -2497,7 +2533,7 @@
         <v>4</v>
       </c>
       <c r="B15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C15" s="3">
         <v>1</v>
@@ -2549,7 +2585,7 @@
         <v>4</v>
       </c>
       <c r="B17" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C17" s="3">
         <v>2</v>
@@ -2575,7 +2611,7 @@
         <v>4</v>
       </c>
       <c r="B18" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C18" s="3">
         <v>1</v>
@@ -2601,7 +2637,7 @@
         <v>4</v>
       </c>
       <c r="B19" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C19" s="3">
         <v>1</v>
@@ -3225,7 +3261,7 @@
         <v>53</v>
       </c>
       <c r="B43" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C43" s="3">
         <v>5</v>
@@ -3234,13 +3270,16 @@
         <f>VLOOKUP(C43,Points!$A$1:$C$6,3,FALSE)</f>
         <v>32</v>
       </c>
+      <c r="E43" t="b">
+        <v>1</v>
+      </c>
       <c r="F43">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G43">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>0</v>
+        <v>32</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -3248,7 +3287,7 @@
         <v>53</v>
       </c>
       <c r="B44" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C44" s="3">
         <v>5</v>
@@ -3257,13 +3296,16 @@
         <f>VLOOKUP(C44,Points!$A$1:$C$6,3,FALSE)</f>
         <v>32</v>
       </c>
+      <c r="E44" t="b">
+        <v>1</v>
+      </c>
       <c r="F44">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G44">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>0</v>
+        <v>32</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -3280,13 +3322,16 @@
         <f>VLOOKUP(C45,Points!$A$1:$C$6,3,FALSE)</f>
         <v>8</v>
       </c>
+      <c r="E45" t="b">
+        <v>1</v>
+      </c>
       <c r="F45">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G45">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -3395,7 +3440,7 @@
         <v>56</v>
       </c>
       <c r="B50" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C50" s="3">
         <v>2</v>
@@ -3421,7 +3466,7 @@
         <v>56</v>
       </c>
       <c r="B51" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C51" s="3">
         <v>2</v>
@@ -3522,7 +3567,7 @@
         <v>56</v>
       </c>
       <c r="B55" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C55" s="3">
         <v>2</v>
@@ -3721,7 +3766,7 @@
         <v>69</v>
       </c>
       <c r="B63" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C63" s="3">
         <v>5</v>
@@ -3730,21 +3775,24 @@
         <f>VLOOKUP(C63,Points!$A$1:$C$6,3,FALSE)</f>
         <v>32</v>
       </c>
+      <c r="E63" t="b">
+        <v>1</v>
+      </c>
       <c r="F63">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G63">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>0</v>
+        <v>32</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B64" t="s">
-        <v>139</v>
+        <v>73</v>
       </c>
       <c r="C64" s="3">
         <v>5</v>
@@ -3753,13 +3801,16 @@
         <f>VLOOKUP(C64,Points!$A$1:$C$6,3,FALSE)</f>
         <v>32</v>
       </c>
+      <c r="E64" t="b">
+        <v>1</v>
+      </c>
       <c r="F64">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G64">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>0</v>
+        <v>32</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
@@ -3767,7 +3818,7 @@
         <v>72</v>
       </c>
       <c r="B65" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C65" s="3">
         <v>5</v>
@@ -3793,25 +3844,25 @@
         <v>72</v>
       </c>
       <c r="B66" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C66" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D66" s="3">
         <f>VLOOKUP(C66,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="E66" t="b">
         <v>1</v>
       </c>
       <c r="F66">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G66">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>32</v>
+        <v>16</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
@@ -3819,51 +3870,51 @@
         <v>72</v>
       </c>
       <c r="B67" t="s">
-        <v>75</v>
+        <v>124</v>
       </c>
       <c r="C67" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D67" s="3">
         <f>VLOOKUP(C67,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="E67" t="b">
         <v>1</v>
       </c>
       <c r="F67">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G67">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>16</v>
+        <v>32</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="B68" t="s">
-        <v>125</v>
+        <v>77</v>
       </c>
       <c r="C68" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D68" s="3">
         <f>VLOOKUP(C68,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="E68" t="b">
         <v>1</v>
       </c>
       <c r="F68">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G68">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>32</v>
+        <v>16</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
@@ -3871,51 +3922,51 @@
         <v>76</v>
       </c>
       <c r="B69" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C69" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D69" s="3">
         <f>VLOOKUP(C69,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="E69" t="b">
         <v>1</v>
       </c>
       <c r="F69">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G69">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>16</v>
+        <v>32</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B70" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C70" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D70" s="3">
         <f>VLOOKUP(C70,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="E70" t="b">
         <v>1</v>
       </c>
       <c r="F70">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G70">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>32</v>
+        <v>16</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
@@ -3926,11 +3977,11 @@
         <v>81</v>
       </c>
       <c r="C71" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D71" s="3">
         <f>VLOOKUP(C71,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="F71">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
@@ -3946,25 +3997,25 @@
         <v>79</v>
       </c>
       <c r="B72" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C72" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D72" s="3">
         <f>VLOOKUP(C72,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="E72" t="b">
         <v>1</v>
       </c>
       <c r="F72">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G72">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>16</v>
+        <v>32</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
@@ -3972,79 +4023,85 @@
         <v>79</v>
       </c>
       <c r="B73" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C73" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D73" s="3">
         <f>VLOOKUP(C73,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>16</v>
+        <v>32</v>
+      </c>
+      <c r="E73" t="b">
+        <v>1</v>
       </c>
       <c r="F73">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G73">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>0</v>
+        <v>32</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="B74" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C74" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D74" s="3">
         <f>VLOOKUP(C74,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="E74" t="b">
         <v>1</v>
       </c>
       <c r="F74">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G74">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>32</v>
+        <v>16</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="B75" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C75" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D75" s="3">
         <f>VLOOKUP(C75,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>32</v>
+        <v>16</v>
+      </c>
+      <c r="E75" t="b">
+        <v>1</v>
       </c>
       <c r="F75">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G75">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B76" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C76" s="3">
         <v>3</v>
@@ -4067,10 +4124,10 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B77" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C77" s="3">
         <v>3</v>
@@ -4093,69 +4150,63 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>85</v>
+        <v>127</v>
       </c>
       <c r="B78" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="C78" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D78" s="3">
         <f>VLOOKUP(C78,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>16</v>
-      </c>
-      <c r="E78" t="b">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F78">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G78">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>85</v>
+        <v>127</v>
       </c>
       <c r="B79" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="C79" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D79" s="3">
         <f>VLOOKUP(C79,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>16</v>
-      </c>
-      <c r="E79" t="b">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F79">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G79">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B80" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C80" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D80" s="3">
         <f>VLOOKUP(C80,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="F80">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
@@ -4168,17 +4219,17 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B81" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C81" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D81" s="3">
         <f>VLOOKUP(C81,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="F81">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
@@ -4191,10 +4242,10 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
+        <v>127</v>
+      </c>
+      <c r="B82" t="s">
         <v>128</v>
-      </c>
-      <c r="B82" t="s">
-        <v>98</v>
       </c>
       <c r="C82" s="3">
         <v>3</v>
@@ -4214,7 +4265,7 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B83" t="s">
         <v>99</v>
@@ -4237,17 +4288,17 @@
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B84" t="s">
-        <v>129</v>
+        <v>100</v>
       </c>
       <c r="C84" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D84" s="3">
         <f>VLOOKUP(C84,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="F84">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
@@ -4260,17 +4311,17 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B85" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C85" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D85" s="3">
         <f>VLOOKUP(C85,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="F85">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
@@ -4283,17 +4334,17 @@
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B86" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="C86" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D86" s="3">
         <f>VLOOKUP(C86,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="F86">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
@@ -4306,17 +4357,17 @@
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B87" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="C87" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D87" s="3">
         <f>VLOOKUP(C87,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="F87">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
@@ -4329,10 +4380,10 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B88" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C88" s="3">
         <v>3</v>
@@ -4352,10 +4403,10 @@
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
+        <v>125</v>
+      </c>
+      <c r="B89" t="s">
         <v>126</v>
-      </c>
-      <c r="B89" t="s">
-        <v>91</v>
       </c>
       <c r="C89" s="3">
         <v>3</v>
@@ -4375,7 +4426,7 @@
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B90" t="s">
         <v>92</v>
@@ -4398,17 +4449,17 @@
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B91" t="s">
-        <v>127</v>
+        <v>93</v>
       </c>
       <c r="C91" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D91" s="3">
         <f>VLOOKUP(C91,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="F91">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
@@ -4421,17 +4472,17 @@
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B92" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C92" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D92" s="3">
         <f>VLOOKUP(C92,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="F92">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
@@ -4444,33 +4495,36 @@
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
       <c r="B93" t="s">
-        <v>94</v>
+        <v>139</v>
       </c>
       <c r="C93" s="3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D93" s="3">
         <f>VLOOKUP(C93,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>4</v>
+        <v>32</v>
+      </c>
+      <c r="E93" t="b">
+        <v>1</v>
       </c>
       <c r="F93">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G93">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>0</v>
+        <v>32</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
       <c r="B94" t="s">
-        <v>95</v>
+        <v>140</v>
       </c>
       <c r="C94" s="3">
         <v>1</v>
@@ -4479,44 +4533,47 @@
         <f>VLOOKUP(C94,Points!$A$1:$C$6,3,FALSE)</f>
         <v>4</v>
       </c>
+      <c r="E94" t="b">
+        <v>1</v>
+      </c>
       <c r="F94">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G94">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B95" t="s">
         <v>141</v>
       </c>
       <c r="C95" s="3">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D95" s="3">
         <f>VLOOKUP(C95,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="E95" t="b">
         <v>1</v>
       </c>
       <c r="F95">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G95">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>32</v>
+        <v>4</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B96" t="s">
         <v>142</v>
@@ -4542,7 +4599,7 @@
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B97" t="s">
         <v>143</v>
@@ -4568,33 +4625,33 @@
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B98" t="s">
         <v>144</v>
       </c>
       <c r="C98" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D98" s="3">
         <f>VLOOKUP(C98,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="E98" t="b">
         <v>1</v>
       </c>
       <c r="F98">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G98">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>4</v>
+        <v>16</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B99" t="s">
         <v>145</v>
@@ -4620,33 +4677,33 @@
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B100" t="s">
         <v>146</v>
       </c>
       <c r="C100" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D100" s="3">
         <f>VLOOKUP(C100,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="E100" t="b">
         <v>1</v>
       </c>
       <c r="F100">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G100">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>16</v>
+        <v>4</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B101" t="s">
         <v>147</v>
@@ -4672,7 +4729,7 @@
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B102" t="s">
         <v>148</v>
@@ -4698,7 +4755,7 @@
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B103" t="s">
         <v>149</v>
@@ -4724,7 +4781,7 @@
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B104" t="s">
         <v>150</v>
@@ -4750,7 +4807,7 @@
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B105" t="s">
         <v>151</v>
@@ -4776,7 +4833,7 @@
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B106" t="s">
         <v>152</v>
@@ -4802,7 +4859,7 @@
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B107" t="s">
         <v>153</v>
@@ -4828,7 +4885,7 @@
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B108" t="s">
         <v>154</v>
@@ -4854,33 +4911,33 @@
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B109" t="s">
         <v>155</v>
       </c>
       <c r="C109" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D109" s="3">
         <f>VLOOKUP(C109,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E109" t="b">
         <v>1</v>
       </c>
       <c r="F109">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G109">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B110" t="s">
         <v>156</v>
@@ -4906,33 +4963,30 @@
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B111" t="s">
         <v>157</v>
       </c>
       <c r="C111" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D111" s="3">
         <f>VLOOKUP(C111,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>8</v>
-      </c>
-      <c r="E111" t="b">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F111">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G111">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B112" t="s">
         <v>158</v>
@@ -4944,21 +4998,18 @@
         <f>VLOOKUP(C112,Points!$A$1:$C$6,3,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="E112" t="b">
-        <v>1</v>
-      </c>
       <c r="F112">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G112">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B113" t="s">
         <v>159</v>
@@ -4981,17 +5032,17 @@
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B114" t="s">
         <v>160</v>
       </c>
       <c r="C114" s="3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D114" s="3">
         <f>VLOOKUP(C114,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="F114">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
@@ -5004,17 +5055,17 @@
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B115" t="s">
         <v>161</v>
       </c>
       <c r="C115" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D115" s="3">
         <f>VLOOKUP(C115,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="F115">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
@@ -5027,79 +5078,82 @@
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B116" t="s">
         <v>162</v>
       </c>
       <c r="C116" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D116" s="3">
         <f>VLOOKUP(C116,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>32</v>
+        <v>16</v>
+      </c>
+      <c r="E116" t="b">
+        <v>1</v>
       </c>
       <c r="F116">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G116">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B117" t="s">
         <v>163</v>
       </c>
       <c r="C117" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D117" s="3">
         <f>VLOOKUP(C117,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>16</v>
+        <v>4</v>
+      </c>
+      <c r="E117" t="b">
+        <v>1</v>
       </c>
       <c r="F117">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G117">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B118" t="s">
         <v>164</v>
       </c>
       <c r="C118" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D118" s="3">
         <f>VLOOKUP(C118,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>16</v>
-      </c>
-      <c r="E118" t="b">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F118">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G118">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B119" t="s">
         <v>165</v>
@@ -5111,96 +5165,99 @@
         <f>VLOOKUP(C119,Points!$A$1:$C$6,3,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="E119" t="b">
-        <v>1</v>
-      </c>
       <c r="F119">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G119">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B120" t="s">
         <v>166</v>
       </c>
       <c r="C120" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D120" s="3">
         <f>VLOOKUP(C120,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>4</v>
+        <v>8</v>
+      </c>
+      <c r="E120" t="b">
+        <v>1</v>
       </c>
       <c r="F120">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G120">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B121" t="s">
         <v>167</v>
       </c>
       <c r="C121" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D121" s="3">
         <f>VLOOKUP(C121,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>4</v>
+        <v>8</v>
+      </c>
+      <c r="E121" t="b">
+        <v>1</v>
       </c>
       <c r="F121">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G121">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B122" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="C122" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D122" s="3">
         <f>VLOOKUP(C122,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E122" t="b">
         <v>1</v>
       </c>
       <c r="F122">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G122">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B123" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C123" s="3">
         <v>2</v>
@@ -5223,33 +5280,30 @@
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B124" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="C124" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D124" s="3">
         <f>VLOOKUP(C124,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>4</v>
-      </c>
-      <c r="E124" t="b">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F124">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G124">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B125" t="s">
         <v>170</v>
@@ -5261,96 +5315,96 @@
         <f>VLOOKUP(C125,Points!$A$1:$C$6,3,FALSE)</f>
         <v>8</v>
       </c>
-      <c r="E125" t="b">
-        <v>1</v>
-      </c>
       <c r="F125">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G125">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B126" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="C126" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D126" s="3">
         <f>VLOOKUP(C126,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="E126" t="b">
+        <v>1</v>
       </c>
       <c r="F126">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G126">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>140</v>
+        <v>64</v>
       </c>
       <c r="B127" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C127" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D127" s="3">
         <f>VLOOKUP(C127,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="E127" t="b">
+        <v>1</v>
       </c>
       <c r="F127">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G127">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>140</v>
+        <v>56</v>
       </c>
       <c r="B128" t="s">
         <v>176</v>
       </c>
       <c r="C128" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D128" s="3">
         <f>VLOOKUP(C128,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>4</v>
-      </c>
-      <c r="E128" t="b">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="F128">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G128">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>64</v>
+        <v>177</v>
       </c>
       <c r="B129" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C129" s="3">
         <v>1</v>
@@ -5359,54 +5413,54 @@
         <f>VLOOKUP(C129,Points!$A$1:$C$6,3,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="E129" t="b">
-        <v>1</v>
-      </c>
       <c r="F129">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G129">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>56</v>
+        <v>138</v>
       </c>
       <c r="B130" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C130" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D130" s="3">
         <f>VLOOKUP(C130,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>16</v>
+        <v>4</v>
+      </c>
+      <c r="E130" t="b">
+        <v>1</v>
       </c>
       <c r="F130">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G130">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>179</v>
+        <v>138</v>
       </c>
       <c r="B131" t="s">
         <v>180</v>
       </c>
       <c r="C131" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D131" s="3">
         <f>VLOOKUP(C131,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="F131">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
@@ -5419,7 +5473,7 @@
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B132" t="s">
         <v>181</v>
@@ -5442,63 +5496,69 @@
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B133" t="s">
         <v>182</v>
       </c>
       <c r="C133" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D133" s="3">
         <f>VLOOKUP(C133,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>16</v>
+        <v>4</v>
+      </c>
+      <c r="E133" t="b">
+        <v>1</v>
       </c>
       <c r="F133">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G133">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B134" t="s">
         <v>183</v>
       </c>
       <c r="C134" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D134" s="3">
         <f>VLOOKUP(C134,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>4</v>
+        <v>8</v>
+      </c>
+      <c r="E134" t="b">
+        <v>1</v>
       </c>
       <c r="F134">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G134">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B135" t="s">
         <v>184</v>
       </c>
       <c r="C135" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D135" s="3">
         <f>VLOOKUP(C135,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="F135">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
@@ -5511,43 +5571,40 @@
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>140</v>
+        <v>53</v>
       </c>
       <c r="B136" t="s">
-        <v>185</v>
+        <v>55</v>
       </c>
       <c r="C136" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D136" s="3">
         <f>VLOOKUP(C136,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>8</v>
-      </c>
-      <c r="E136" t="b">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F136">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G136">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>140</v>
+        <v>53</v>
       </c>
       <c r="B137" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C137" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D137" s="3">
         <f>VLOOKUP(C137,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="F137">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
@@ -5560,180 +5617,183 @@
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
       <c r="B138" t="s">
-        <v>55</v>
+        <v>190</v>
       </c>
       <c r="C138" s="3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D138" s="3">
         <f>VLOOKUP(C138,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>4</v>
+        <v>32</v>
+      </c>
+      <c r="E138" t="b">
+        <v>1</v>
       </c>
       <c r="F138">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G138">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>0</v>
+        <v>32</v>
       </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>53</v>
+        <v>72</v>
       </c>
       <c r="B139" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="C139" s="3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D139" s="3">
         <f>VLOOKUP(C139,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>4</v>
+        <v>32</v>
+      </c>
+      <c r="E139" t="b">
+        <v>1</v>
       </c>
       <c r="F139">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G139">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>0</v>
+        <v>32</v>
       </c>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>69</v>
+        <v>138</v>
       </c>
       <c r="B140" t="s">
         <v>192</v>
       </c>
       <c r="C140" s="3">
-        <v>5</v>
-      </c>
-      <c r="D140" s="15">
+        <v>1</v>
+      </c>
+      <c r="D140" s="3">
         <f>VLOOKUP(C140,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="E140" t="b">
         <v>1</v>
       </c>
-      <c r="F140" s="16">
-        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>5</v>
-      </c>
-      <c r="G140" s="16">
-        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>32</v>
+      <c r="F140">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>1</v>
+      </c>
+      <c r="G140">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
+        <v>4</v>
       </c>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>72</v>
+        <v>138</v>
       </c>
       <c r="B141" t="s">
         <v>193</v>
       </c>
       <c r="C141" s="3">
-        <v>5</v>
-      </c>
-      <c r="D141" s="15">
+        <v>1</v>
+      </c>
+      <c r="D141" s="3">
         <f>VLOOKUP(C141,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="E141" t="b">
         <v>1</v>
       </c>
-      <c r="F141" s="16">
-        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>5</v>
-      </c>
-      <c r="G141" s="16">
-        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>32</v>
+      <c r="F141">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>1</v>
+      </c>
+      <c r="G141">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
+        <v>4</v>
       </c>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B142" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="C142" s="3">
-        <v>1</v>
-      </c>
-      <c r="D142" s="15">
+        <v>3</v>
+      </c>
+      <c r="D142" s="3">
         <f>VLOOKUP(C142,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>4</v>
-      </c>
-      <c r="E142" t="b">
-        <v>1</v>
-      </c>
-      <c r="F142" s="16">
-        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>1</v>
-      </c>
-      <c r="G142" s="16">
-        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>4</v>
+        <v>16</v>
+      </c>
+      <c r="F142">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="G142">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B143" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="C143" s="3">
         <v>1</v>
       </c>
-      <c r="D143" s="15">
+      <c r="D143" s="3">
         <f>VLOOKUP(C143,Points!$A$1:$C$6,3,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="E143" t="b">
-        <v>1</v>
-      </c>
-      <c r="F143" s="16">
-        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>1</v>
-      </c>
-      <c r="G143" s="16">
-        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>4</v>
+      <c r="F143">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="G143">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B144" t="s">
         <v>188</v>
       </c>
       <c r="C144" s="3">
-        <v>3</v>
-      </c>
-      <c r="D144" s="15">
+        <v>1</v>
+      </c>
+      <c r="D144" s="3">
         <f>VLOOKUP(C144,Points!$A$1:$C$6,3,FALSE)</f>
-        <v>16</v>
-      </c>
-      <c r="F144" s="16">
-        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
-      </c>
-      <c r="G144" s="16">
-        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="E144" t="b">
+        <v>1</v>
+      </c>
+      <c r="F144">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>1</v>
+      </c>
+      <c r="G144">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
+        <v>4</v>
       </c>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B145" t="s">
         <v>189</v>
@@ -5741,25 +5801,28 @@
       <c r="C145" s="3">
         <v>1</v>
       </c>
-      <c r="D145" s="15">
+      <c r="D145" s="3">
         <f>VLOOKUP(C145,Points!$A$1:$C$6,3,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="F145" s="16">
-        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
-      </c>
-      <c r="G145" s="16">
-        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>0</v>
+      <c r="E145" t="b">
+        <v>1</v>
+      </c>
+      <c r="F145">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>1</v>
+      </c>
+      <c r="G145">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
+        <v>4</v>
       </c>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B146" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="C146" s="3">
         <v>1</v>
@@ -5768,21 +5831,24 @@
         <f>VLOOKUP(C146,Points!$A$1:$C$6,3,FALSE)</f>
         <v>4</v>
       </c>
+      <c r="E146" t="b">
+        <v>1</v>
+      </c>
       <c r="F146" s="16">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G146" s="16">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B147" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="C147" s="3">
         <v>1</v>
@@ -5791,148 +5857,497 @@
         <f>VLOOKUP(C147,Points!$A$1:$C$6,3,FALSE)</f>
         <v>4</v>
       </c>
+      <c r="E147" t="b">
+        <v>1</v>
+      </c>
       <c r="F147" s="16">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G147" s="16">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>0</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>138</v>
+      </c>
+      <c r="B148" t="s">
+        <v>198</v>
+      </c>
+      <c r="C148" s="3">
+        <v>3</v>
+      </c>
+      <c r="D148" s="15">
+        <f>VLOOKUP(C148,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>16</v>
+      </c>
+      <c r="E148" t="b">
+        <v>1</v>
+      </c>
+      <c r="F148" s="16">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>3</v>
+      </c>
+      <c r="G148" s="16">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
+        <v>16</v>
       </c>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A149" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="B149" s="4"/>
-      <c r="C149" s="5">
-        <f>SUM(C2:C148)</f>
-        <v>357</v>
-      </c>
-      <c r="D149" s="5">
-        <f>SUM(D2:D148)</f>
-        <v>1896</v>
-      </c>
-      <c r="F149" s="4">
-        <f>SUM(F2:F148)</f>
-        <v>233</v>
-      </c>
-      <c r="G149" s="4">
-        <f>SUM(G2:G148)</f>
-        <v>1232</v>
+      <c r="A149" t="s">
+        <v>138</v>
+      </c>
+      <c r="B149" t="s">
+        <v>199</v>
+      </c>
+      <c r="C149" s="3">
+        <v>1</v>
+      </c>
+      <c r="D149" s="15">
+        <f>VLOOKUP(C149,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="E149" t="b">
+        <v>1</v>
+      </c>
+      <c r="F149" s="16">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>1</v>
+      </c>
+      <c r="G149" s="16">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
+        <v>4</v>
       </c>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A150" s="6"/>
-      <c r="B150" s="4"/>
-      <c r="C150" s="5"/>
-      <c r="D150" s="5"/>
-      <c r="G150" s="4"/>
+      <c r="A150" t="s">
+        <v>138</v>
+      </c>
+      <c r="B150" t="s">
+        <v>200</v>
+      </c>
+      <c r="C150" s="3">
+        <v>1</v>
+      </c>
+      <c r="D150" s="15">
+        <f>VLOOKUP(C150,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="E150" t="b">
+        <v>1</v>
+      </c>
+      <c r="F150" s="16">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>1</v>
+      </c>
+      <c r="G150" s="16">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
+        <v>4</v>
+      </c>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A151" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="B151" s="11">
-        <f ca="1">B153+B152</f>
-        <v>125.33766233766234</v>
-      </c>
-      <c r="D151" s="7"/>
+      <c r="A151" t="s">
+        <v>138</v>
+      </c>
+      <c r="B151" t="s">
+        <v>201</v>
+      </c>
+      <c r="C151" s="3">
+        <v>1</v>
+      </c>
+      <c r="D151" s="15">
+        <f>VLOOKUP(C151,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="E151" t="b">
+        <v>1</v>
+      </c>
+      <c r="F151" s="16">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>1</v>
+      </c>
+      <c r="G151" s="16">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
+        <v>4</v>
+      </c>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A152" s="6" t="s">
+      <c r="A152" t="s">
+        <v>138</v>
+      </c>
+      <c r="B152" t="s">
+        <v>163</v>
+      </c>
+      <c r="C152" s="3">
+        <v>1</v>
+      </c>
+      <c r="D152" s="15">
+        <f>VLOOKUP(C152,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="E152" t="b">
+        <v>1</v>
+      </c>
+      <c r="F152" s="16">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>1</v>
+      </c>
+      <c r="G152" s="16">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>138</v>
+      </c>
+      <c r="B153" t="s">
+        <v>183</v>
+      </c>
+      <c r="C153" s="3">
+        <v>2</v>
+      </c>
+      <c r="D153" s="15">
+        <f>VLOOKUP(C153,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>8</v>
+      </c>
+      <c r="E153" t="b">
+        <v>1</v>
+      </c>
+      <c r="F153" s="16">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>2</v>
+      </c>
+      <c r="G153" s="16">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>138</v>
+      </c>
+      <c r="B154" t="s">
+        <v>192</v>
+      </c>
+      <c r="C154" s="3">
+        <v>1</v>
+      </c>
+      <c r="D154" s="15">
+        <f>VLOOKUP(C154,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="E154" t="b">
+        <v>1</v>
+      </c>
+      <c r="F154" s="16">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>1</v>
+      </c>
+      <c r="G154" s="16">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>138</v>
+      </c>
+      <c r="B155" t="s">
+        <v>190</v>
+      </c>
+      <c r="C155" s="3">
+        <v>5</v>
+      </c>
+      <c r="D155" s="15">
+        <f>VLOOKUP(C155,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>32</v>
+      </c>
+      <c r="E155" t="b">
+        <v>1</v>
+      </c>
+      <c r="F155" s="16">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>5</v>
+      </c>
+      <c r="G155" s="16">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>138</v>
+      </c>
+      <c r="B156" t="s">
+        <v>202</v>
+      </c>
+      <c r="C156" s="3">
+        <v>1</v>
+      </c>
+      <c r="D156" s="15">
+        <f>VLOOKUP(C156,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="F156" s="16">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="G156" s="16">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>138</v>
+      </c>
+      <c r="B157" t="s">
+        <v>203</v>
+      </c>
+      <c r="C157" s="3">
+        <v>1</v>
+      </c>
+      <c r="D157" s="15">
+        <f>VLOOKUP(C157,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="F157" s="16">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="G157" s="16">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>138</v>
+      </c>
+      <c r="B158" t="s">
+        <v>204</v>
+      </c>
+      <c r="C158" s="3">
+        <v>1</v>
+      </c>
+      <c r="D158" s="15">
+        <f>VLOOKUP(C158,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="F158" s="16">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="G158" s="16">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>138</v>
+      </c>
+      <c r="B159" t="s">
+        <v>205</v>
+      </c>
+      <c r="C159" s="3">
+        <v>1</v>
+      </c>
+      <c r="D159" s="15">
+        <f>VLOOKUP(C159,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="F159" s="16">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="G159" s="16">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>138</v>
+      </c>
+      <c r="B160" t="s">
+        <v>206</v>
+      </c>
+      <c r="C160" s="3">
+        <v>1</v>
+      </c>
+      <c r="D160" s="15">
+        <f>VLOOKUP(C160,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="F160" s="16">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="G160" s="16">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>138</v>
+      </c>
+      <c r="B161" t="s">
+        <v>207</v>
+      </c>
+      <c r="C161" s="3">
+        <v>1</v>
+      </c>
+      <c r="D161" s="15">
+        <f>VLOOKUP(C161,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="F161" s="16">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>0</v>
+      </c>
+      <c r="G161" s="16">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A163" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="B163" s="4"/>
+      <c r="C163" s="5">
+        <f>SUM(C2:C162)</f>
+        <v>370</v>
+      </c>
+      <c r="D163" s="5">
+        <f>SUM(D2:D162)</f>
+        <v>1940</v>
+      </c>
+      <c r="F163" s="4">
+        <f>SUM(F2:F162)</f>
+        <v>276</v>
+      </c>
+      <c r="G163" s="4">
+        <f>SUM(G2:G162)</f>
+        <v>1468</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A164" s="6"/>
+      <c r="B164" s="4"/>
+      <c r="C164" s="5"/>
+      <c r="D164" s="5"/>
+      <c r="G164" s="4"/>
+    </row>
+    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A165" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="B165" s="11">
+        <f ca="1">B167+B166</f>
+        <v>114.93460490463215</v>
+      </c>
+      <c r="D165" s="7"/>
+    </row>
+    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A166" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="B166" s="11">
+        <f ca="1">(D163-G163)/B173</f>
+        <v>19.934604904632153</v>
+      </c>
+      <c r="D166" s="7"/>
+    </row>
+    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A167" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="B167" s="4">
+        <f ca="1">FLOOR(((TODAY()-Variables!B2)/7),1)</f>
+        <v>95</v>
+      </c>
+      <c r="D167" s="7"/>
+    </row>
+    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A168" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="B168" s="4">
+        <v>33</v>
+      </c>
+      <c r="D168" s="7"/>
+    </row>
+    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A169" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="B169" s="4">
+        <f ca="1">B167-B168</f>
+        <v>62</v>
+      </c>
+      <c r="D169" s="7"/>
+    </row>
+    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A170" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="B152" s="11">
-        <f ca="1">(D149-G149)/B159</f>
-        <v>32.337662337662337</v>
-      </c>
-      <c r="D152" s="7"/>
-    </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A153" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="B153" s="4">
-        <f ca="1">FLOOR(((TODAY()-Variables!B2)/7),1)</f>
-        <v>93</v>
-      </c>
-      <c r="D153" s="7"/>
-    </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A154" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="B154" s="4">
-        <v>33</v>
-      </c>
-      <c r="D154" s="7"/>
-    </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A155" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="B155" s="4">
-        <f ca="1">B153-B154</f>
-        <v>60</v>
-      </c>
-      <c r="D155" s="7"/>
-    </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A156" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="B156" s="12">
+      <c r="B170" s="12">
         <f>Variables!B2</f>
         <v>44892</v>
       </c>
-      <c r="D156" s="7"/>
-    </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A157" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="B157" s="12">
-        <f ca="1">TODAY()+ (B152*7)</f>
-        <v>45770.36363636364</v>
-      </c>
-      <c r="D157" s="9"/>
-    </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A158" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="B158" s="11">
-        <f ca="1">F149/B155</f>
-        <v>3.8833333333333333</v>
-      </c>
-      <c r="F158" s="10"/>
-    </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A159" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="B159" s="13">
-        <f ca="1">G149/B155</f>
-        <v>20.533333333333335</v>
-      </c>
-    </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A160" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="B160" s="11">
-        <f>D149-G149</f>
-        <v>664</v>
-      </c>
-    </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A161" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="B161" s="14">
-        <f>G149/D149</f>
-        <v>0.64978902953586493</v>
+      <c r="D170" s="7"/>
+    </row>
+    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A171" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="B171" s="12">
+        <f ca="1">TODAY()+ (B166*7)</f>
+        <v>45697.542234332424</v>
+      </c>
+      <c r="D171" s="9"/>
+    </row>
+    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A172" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B172" s="11">
+        <f ca="1">F163/B169</f>
+        <v>4.4516129032258061</v>
+      </c>
+      <c r="F172" s="10"/>
+    </row>
+    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A173" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B173" s="13">
+        <f ca="1">G163/B169</f>
+        <v>23.677419354838708</v>
+      </c>
+    </row>
+    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A174" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="B174" s="11">
+        <f>D163-G163</f>
+        <v>472</v>
+      </c>
+    </row>
+    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A175" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="B175" s="14">
+        <f>G163/D163</f>
+        <v>0.75670103092783503</v>
       </c>
     </row>
   </sheetData>
@@ -5946,10 +6361,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77214E7E-2154-4807-A446-0B02AF797AAE}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K30" sqref="K30"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5961,13 +6376,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -6023,6 +6438,17 @@
       </c>
       <c r="C6">
         <v>664</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="8">
+        <v>45558</v>
+      </c>
+      <c r="B7">
+        <v>62</v>
+      </c>
+      <c r="C7">
+        <v>472</v>
       </c>
     </row>
   </sheetData>
@@ -6133,15 +6559,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B2">
         <v>8</v>
@@ -6149,7 +6575,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -6157,7 +6583,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B4">
         <v>10</v>
@@ -6165,7 +6591,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B6" s="4">
         <f>SUM(B2:B4)</f>
@@ -6192,15 +6618,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B2" s="8">
         <v>44892</v>

</xml_diff>

<commit_message>
Update to project status
</commit_message>
<xml_diff>
--- a/Documentation/Design/Estimates.xlsx
+++ b/Documentation/Design/Estimates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_git\BedBrigadeNationalV8\Documentation\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4E87900-C781-4600-BD37-2F6876828EF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93C16D39-7FFC-47CF-9947-C27F3891235C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D27F5AFA-C88C-4A2F-A896-BFED2572A1C7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{D27F5AFA-C88C-4A2F-A896-BFED2572A1C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Estimates" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="229">
   <si>
     <t>Epic</t>
   </si>
@@ -721,6 +721,12 @@
   </si>
   <si>
     <t>Localize Dynamic Content</t>
+  </si>
+  <si>
+    <t>Make EmailQueue into a Background Service</t>
+  </si>
+  <si>
+    <t>Apply String Localization</t>
   </si>
 </sst>
 </file>
@@ -785,7 +791,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -813,6 +819,10 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -948,10 +958,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Burn Down'!$B$2:$B$9</c:f>
+              <c:f>'Burn Down'!$B$2:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>56</c:v>
                 </c:pt>
@@ -976,15 +986,18 @@
                 <c:pt idx="7">
                   <c:v>64</c:v>
                 </c:pt>
+                <c:pt idx="8">
+                  <c:v>65</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Burn Down'!$C$2:$C$9</c:f>
+              <c:f>'Burn Down'!$C$2:$C$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>568</c:v>
                 </c:pt>
@@ -1008,6 +1021,9 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>548</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>524</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1896,8 +1912,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{20A5C34A-BA74-4618-9527-C8C5A4B15239}" name="Table1" displayName="Table1" ref="A1:G180" totalsRowShown="0">
-  <autoFilter ref="A1:G180" xr:uid="{20A5C34A-BA74-4618-9527-C8C5A4B15239}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{20A5C34A-BA74-4618-9527-C8C5A4B15239}" name="Table1" displayName="Table1" ref="A1:G182" totalsRowShown="0">
+  <autoFilter ref="A1:G182" xr:uid="{20A5C34A-BA74-4618-9527-C8C5A4B15239}"/>
   <tableColumns count="7">
     <tableColumn id="2" xr3:uid="{8122BCC0-A9A0-4E8A-97F8-809454E87965}" name="Epic"/>
     <tableColumn id="3" xr3:uid="{62273C57-4035-404E-BD7F-DBE541848AF0}" name="Story"/>
@@ -2214,11 +2230,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F9D3302-E5F0-4E5C-9EB3-B74DDF37DF9D}">
-  <dimension ref="A1:G196"/>
+  <dimension ref="A1:G198"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A168" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B159" sqref="B159:B169"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A173" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E191" sqref="E191"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5735,13 +5751,16 @@
         <f>VLOOKUP(C139,Points!$A$1:$C$6,3,FALSE)</f>
         <v>4</v>
       </c>
+      <c r="E139" t="b">
+        <v>1</v>
+      </c>
       <c r="F139">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G139">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.25">
@@ -6070,13 +6089,16 @@
         <f>VLOOKUP(C152,Points!$A$1:$C$6,3,FALSE)</f>
         <v>4</v>
       </c>
+      <c r="E152" t="b">
+        <v>1</v>
+      </c>
       <c r="F152">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G152">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.25">
@@ -6738,148 +6760,203 @@
         <f>VLOOKUP(C180,Points!$A$1:$C$6,3,FALSE)</f>
         <v>16</v>
       </c>
+      <c r="E180" t="b">
+        <v>1</v>
+      </c>
       <c r="F180">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G180">
         <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A184" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="B184" s="4"/>
-      <c r="C184" s="5">
-        <f>SUM(C2:C183)</f>
-        <v>411</v>
-      </c>
-      <c r="D184" s="5">
-        <f>SUM(D2:D183)</f>
-        <v>2132</v>
-      </c>
-      <c r="F184" s="4">
-        <f>SUM(F2:F183)</f>
-        <v>299</v>
-      </c>
-      <c r="G184" s="4">
-        <f>SUM(G2:G183)</f>
-        <v>1584</v>
-      </c>
-    </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A185" s="6"/>
-      <c r="B185" s="4"/>
-      <c r="C185" s="5"/>
-      <c r="D185" s="5"/>
-      <c r="G185" s="4"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
+        <v>138</v>
+      </c>
+      <c r="B181" t="s">
+        <v>227</v>
+      </c>
+      <c r="C181" s="3">
+        <v>1</v>
+      </c>
+      <c r="D181" s="15">
+        <f>VLOOKUP(C181,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="E181" t="b">
+        <v>1</v>
+      </c>
+      <c r="F181" s="16">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>1</v>
+      </c>
+      <c r="G181" s="16">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
+        <v>173</v>
+      </c>
+      <c r="B182" t="s">
+        <v>228</v>
+      </c>
+      <c r="C182" s="3">
+        <v>3</v>
+      </c>
+      <c r="D182" s="15">
+        <f>VLOOKUP(C182,Points!$A$1:$C$6,3,FALSE)</f>
+        <v>16</v>
+      </c>
+      <c r="E182" t="b">
+        <v>1</v>
+      </c>
+      <c r="F182" s="16">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Points]],0)</f>
+        <v>3</v>
+      </c>
+      <c r="G182" s="16">
+        <f>IF(Table1[[#This Row],[Completed]],Table1[[#This Row],[Estimated Hours]],0)</f>
+        <v>16</v>
+      </c>
     </row>
     <row r="186" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A186" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="B186" s="11">
-        <f ca="1">B188+B187</f>
-        <v>119.14141414141415</v>
-      </c>
-      <c r="D186" s="7"/>
+        <v>102</v>
+      </c>
+      <c r="B186" s="4"/>
+      <c r="C186" s="5">
+        <f>SUM(C2:C185)</f>
+        <v>415</v>
+      </c>
+      <c r="D186" s="5">
+        <f>SUM(D2:D185)</f>
+        <v>2152</v>
+      </c>
+      <c r="F186" s="4">
+        <f>SUM(F2:F185)</f>
+        <v>308</v>
+      </c>
+      <c r="G186" s="4">
+        <f>SUM(G2:G185)</f>
+        <v>1628</v>
+      </c>
     </row>
     <row r="187" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A187" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="B187" s="11">
-        <f ca="1">(D184-G184)/B194</f>
-        <v>22.141414141414142</v>
-      </c>
-      <c r="D187" s="7"/>
+      <c r="A187" s="6"/>
+      <c r="B187" s="4"/>
+      <c r="C187" s="5"/>
+      <c r="D187" s="5"/>
+      <c r="G187" s="4"/>
     </row>
     <row r="188" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A188" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="B188" s="4">
-        <f ca="1">FLOOR(((TODAY()-Variables!B2)/7),1)</f>
-        <v>97</v>
+        <v>107</v>
+      </c>
+      <c r="B188" s="11">
+        <f ca="1">B190+B189</f>
+        <v>118.92137592137593</v>
       </c>
       <c r="D188" s="7"/>
     </row>
     <row r="189" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A189" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="B189" s="4">
-        <v>33</v>
+        <v>119</v>
+      </c>
+      <c r="B189" s="11">
+        <f ca="1">(D186-G186)/B196</f>
+        <v>20.921375921375923</v>
       </c>
       <c r="D189" s="7"/>
     </row>
     <row r="190" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A190" s="6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B190" s="4">
-        <f ca="1">B188-B189</f>
-        <v>64</v>
+        <f ca="1">FLOOR(((TODAY()-Variables!B2)/7),1)</f>
+        <v>98</v>
       </c>
       <c r="D190" s="7"/>
     </row>
     <row r="191" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A191" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="B191" s="4">
+        <v>33</v>
+      </c>
+      <c r="D191" s="7"/>
+    </row>
+    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A192" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="B192" s="4">
+        <f ca="1">B190-B191</f>
+        <v>65</v>
+      </c>
+      <c r="D192" s="7"/>
+    </row>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A193" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="B191" s="12">
+      <c r="B193" s="12">
         <f>Variables!B2</f>
         <v>44892</v>
       </c>
-      <c r="D191" s="7"/>
-    </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A192" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="B192" s="12">
-        <f ca="1">TODAY()+ (B187*7)</f>
-        <v>45726.989898989901</v>
-      </c>
-      <c r="D192" s="9"/>
-    </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A193" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="B193" s="11">
-        <f ca="1">F184/B190</f>
-        <v>4.671875</v>
-      </c>
-      <c r="F193" s="10"/>
+      <c r="D193" s="7"/>
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A194" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="B194" s="13">
-        <f ca="1">G184/B190</f>
-        <v>24.75</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="B194" s="12">
+        <f ca="1">TODAY()+ (B189*7)</f>
+        <v>45725.449631449628</v>
+      </c>
+      <c r="D194" s="9"/>
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A195" s="6" t="s">
-        <v>168</v>
+        <v>116</v>
       </c>
       <c r="B195" s="11">
-        <f>D184-G184</f>
-        <v>548</v>
-      </c>
+        <f ca="1">F186/B192</f>
+        <v>4.7384615384615385</v>
+      </c>
+      <c r="F195" s="10"/>
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A196" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B196" s="13">
+        <f ca="1">G186/B192</f>
+        <v>25.046153846153846</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A197" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="B197" s="11">
+        <f>D186-G186</f>
+        <v>524</v>
+      </c>
+    </row>
+    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A198" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="B196" s="14">
-        <f>G184/D184</f>
-        <v>0.74296435272045025</v>
+      <c r="B198" s="14">
+        <f>G186/D186</f>
+        <v>0.75650557620817849</v>
       </c>
     </row>
   </sheetData>
@@ -6893,15 +6970,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77214E7E-2154-4807-A446-0B02AF797AAE}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -7003,6 +7080,19 @@
       </c>
       <c r="C9">
         <v>548</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="8">
+        <f>A9+7</f>
+        <v>45579</v>
+      </c>
+      <c r="B10">
+        <f>B9+1</f>
+        <v>65</v>
+      </c>
+      <c r="C10">
+        <v>524</v>
       </c>
     </row>
   </sheetData>

</xml_diff>